<commit_message>
modificacion en carga titular e ingreso
</commit_message>
<xml_diff>
--- a/Excel/Carga DB Postgres/Ingreso - cargado.xlsx
+++ b/Excel/Carga DB Postgres/Ingreso - cargado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="350">
   <si>
     <t>idingreso</t>
   </si>
@@ -1405,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Y92" sqref="Y91:Y92"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1529,11 +1529,11 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
@@ -1559,6 +1559,9 @@
       <c r="M2" t="s">
         <v>318</v>
       </c>
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
       <c r="O2" t="s">
         <v>334</v>
       </c>
@@ -1567,16 +1570,19 @@
       </c>
       <c r="Q2">
         <f ca="1">RANDBETWEEN(100,10000)</f>
-        <v>9703</v>
+        <v>5171</v>
       </c>
       <c r="R2">
         <f ca="1">RANDBETWEEN(1,153)</f>
-        <v>127</v>
+        <v>39</v>
       </c>
       <c r="S2" t="s">
         <v>38</v>
       </c>
       <c r="T2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z2" t="s">
         <v>38</v>
       </c>
       <c r="AA2" s="2" t="s">
@@ -1587,7 +1593,7 @@
       </c>
       <c r="AC2">
         <f ca="1">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD2">
         <v>1</v>
@@ -1602,11 +1608,11 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C66" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D66" ca="1" si="1">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -1632,6 +1638,9 @@
       <c r="M3" t="s">
         <v>319</v>
       </c>
+      <c r="N3" t="s">
+        <v>38</v>
+      </c>
       <c r="O3" t="s">
         <v>335</v>
       </c>
@@ -1640,16 +1649,19 @@
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q66" ca="1" si="2">RANDBETWEEN(100,10000)</f>
-        <v>3242</v>
+        <v>1864</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R66" ca="1" si="3">RANDBETWEEN(1,153)</f>
-        <v>125</v>
+        <v>10</v>
       </c>
       <c r="S3" t="s">
         <v>38</v>
       </c>
       <c r="T3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" t="s">
         <v>38</v>
       </c>
       <c r="AA3" s="2" t="s">
@@ -1675,11 +1687,11 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>41</v>
@@ -1705,6 +1717,9 @@
       <c r="M4" t="s">
         <v>320</v>
       </c>
+      <c r="N4" t="s">
+        <v>38</v>
+      </c>
       <c r="O4" t="s">
         <v>336</v>
       </c>
@@ -1713,16 +1728,19 @@
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="2"/>
-        <v>7362</v>
+        <v>3144</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="3"/>
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="S4" t="s">
         <v>38</v>
       </c>
       <c r="T4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z4" t="s">
         <v>38</v>
       </c>
       <c r="AA4" s="2" t="s">
@@ -1733,7 +1751,7 @@
       </c>
       <c r="AC4">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD4">
         <v>1</v>
@@ -1748,11 +1766,11 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
         <v>42</v>
@@ -1778,6 +1796,9 @@
       <c r="M5" t="s">
         <v>321</v>
       </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
       <c r="O5" t="s">
         <v>337</v>
       </c>
@@ -1786,16 +1807,19 @@
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="2"/>
-        <v>2764</v>
+        <v>3227</v>
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="S5" t="s">
         <v>38</v>
       </c>
       <c r="T5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z5" t="s">
         <v>38</v>
       </c>
       <c r="AA5" s="2" t="s">
@@ -1806,7 +1830,7 @@
       </c>
       <c r="AC5">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD5">
         <v>1</v>
@@ -1825,7 +1849,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>43</v>
@@ -1851,6 +1875,9 @@
       <c r="M6" t="s">
         <v>322</v>
       </c>
+      <c r="N6" t="s">
+        <v>38</v>
+      </c>
       <c r="O6" t="s">
         <v>338</v>
       </c>
@@ -1859,16 +1886,19 @@
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="2"/>
-        <v>5251</v>
+        <v>4592</v>
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="3"/>
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="S6" t="s">
         <v>38</v>
       </c>
       <c r="T6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z6" t="s">
         <v>38</v>
       </c>
       <c r="AA6" s="2" t="s">
@@ -1894,11 +1924,11 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
@@ -1924,6 +1954,9 @@
       <c r="M7" t="s">
         <v>323</v>
       </c>
+      <c r="N7" t="s">
+        <v>38</v>
+      </c>
       <c r="O7" t="s">
         <v>339</v>
       </c>
@@ -1932,16 +1965,19 @@
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="2"/>
-        <v>2912</v>
+        <v>3581</v>
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="3"/>
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="S7" t="s">
         <v>38</v>
       </c>
       <c r="T7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z7" t="s">
         <v>38</v>
       </c>
       <c r="AA7" s="2" t="s">
@@ -1967,11 +2003,11 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
         <v>45</v>
@@ -1997,6 +2033,9 @@
       <c r="M8" t="s">
         <v>324</v>
       </c>
+      <c r="N8" t="s">
+        <v>38</v>
+      </c>
       <c r="O8" t="s">
         <v>340</v>
       </c>
@@ -2005,16 +2044,19 @@
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="2"/>
-        <v>8414</v>
+        <v>1903</v>
       </c>
       <c r="R8">
         <f t="shared" ca="1" si="3"/>
-        <v>131</v>
+        <v>5</v>
       </c>
       <c r="S8" t="s">
         <v>38</v>
       </c>
       <c r="T8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z8" t="s">
         <v>38</v>
       </c>
       <c r="AA8" s="2" t="s">
@@ -2040,11 +2082,11 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
         <v>46</v>
@@ -2070,6 +2112,9 @@
       <c r="M9" t="s">
         <v>325</v>
       </c>
+      <c r="N9" t="s">
+        <v>38</v>
+      </c>
       <c r="O9" t="s">
         <v>341</v>
       </c>
@@ -2078,16 +2123,19 @@
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="2"/>
-        <v>5944</v>
+        <v>7497</v>
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="3"/>
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="S9" t="s">
         <v>38</v>
       </c>
       <c r="T9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z9" t="s">
         <v>38</v>
       </c>
       <c r="AA9" s="2" t="s">
@@ -2098,7 +2146,7 @@
       </c>
       <c r="AC9">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD9">
         <v>1</v>
@@ -2113,7 +2161,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
@@ -2143,6 +2191,9 @@
       <c r="M10" t="s">
         <v>326</v>
       </c>
+      <c r="N10" t="s">
+        <v>38</v>
+      </c>
       <c r="O10" t="s">
         <v>342</v>
       </c>
@@ -2151,16 +2202,19 @@
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="2"/>
-        <v>8003</v>
+        <v>6207</v>
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>119</v>
       </c>
       <c r="S10" t="s">
         <v>38</v>
       </c>
       <c r="T10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z10" t="s">
         <v>38</v>
       </c>
       <c r="AA10" s="2" t="s">
@@ -2186,11 +2240,11 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>48</v>
@@ -2216,6 +2270,9 @@
       <c r="M11" t="s">
         <v>327</v>
       </c>
+      <c r="N11" t="s">
+        <v>38</v>
+      </c>
       <c r="O11" t="s">
         <v>343</v>
       </c>
@@ -2224,16 +2281,19 @@
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="2"/>
-        <v>4139</v>
+        <v>8256</v>
       </c>
       <c r="R11">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="S11" t="s">
         <v>38</v>
       </c>
       <c r="T11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z11" t="s">
         <v>38</v>
       </c>
       <c r="AA11" s="2" t="s">
@@ -2244,7 +2304,7 @@
       </c>
       <c r="AC11">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD11">
         <v>1</v>
@@ -2259,7 +2319,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
@@ -2289,6 +2349,9 @@
       <c r="M12" t="s">
         <v>328</v>
       </c>
+      <c r="N12" t="s">
+        <v>38</v>
+      </c>
       <c r="O12" t="s">
         <v>344</v>
       </c>
@@ -2297,16 +2360,19 @@
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="2"/>
-        <v>8500</v>
+        <v>6084</v>
       </c>
       <c r="R12">
         <f t="shared" ca="1" si="3"/>
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="S12" t="s">
         <v>38</v>
       </c>
       <c r="T12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z12" t="s">
         <v>38</v>
       </c>
       <c r="AA12" s="2" t="s">
@@ -2317,7 +2383,7 @@
       </c>
       <c r="AC12">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD12">
         <v>1</v>
@@ -2332,11 +2398,11 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
         <v>50</v>
@@ -2362,6 +2428,9 @@
       <c r="M13" t="s">
         <v>329</v>
       </c>
+      <c r="N13" t="s">
+        <v>38</v>
+      </c>
       <c r="O13" t="s">
         <v>345</v>
       </c>
@@ -2370,16 +2439,19 @@
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="2"/>
-        <v>5805</v>
+        <v>4620</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="3"/>
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="S13" t="s">
         <v>38</v>
       </c>
       <c r="T13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z13" t="s">
         <v>38</v>
       </c>
       <c r="AA13" s="2" t="s">
@@ -2405,7 +2477,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
@@ -2435,6 +2507,9 @@
       <c r="M14" t="s">
         <v>330</v>
       </c>
+      <c r="N14" t="s">
+        <v>38</v>
+      </c>
       <c r="O14" t="s">
         <v>346</v>
       </c>
@@ -2443,16 +2518,19 @@
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="2"/>
-        <v>4534</v>
+        <v>7272</v>
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="3"/>
-        <v>130</v>
+        <v>16</v>
       </c>
       <c r="S14" t="s">
         <v>38</v>
       </c>
       <c r="T14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z14" t="s">
         <v>38</v>
       </c>
       <c r="AA14" s="2" t="s">
@@ -2478,11 +2556,11 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
         <v>52</v>
@@ -2508,6 +2586,9 @@
       <c r="M15" t="s">
         <v>331</v>
       </c>
+      <c r="N15" t="s">
+        <v>38</v>
+      </c>
       <c r="O15" t="s">
         <v>347</v>
       </c>
@@ -2516,16 +2597,19 @@
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="2"/>
-        <v>1139</v>
+        <v>8338</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="3"/>
-        <v>119</v>
+        <v>5</v>
       </c>
       <c r="S15" t="s">
         <v>38</v>
       </c>
       <c r="T15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z15" t="s">
         <v>38</v>
       </c>
       <c r="AA15" s="2" t="s">
@@ -2551,11 +2635,11 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E16" t="s">
         <v>53</v>
@@ -2581,6 +2665,9 @@
       <c r="M16" t="s">
         <v>332</v>
       </c>
+      <c r="N16" t="s">
+        <v>38</v>
+      </c>
       <c r="O16" t="s">
         <v>348</v>
       </c>
@@ -2589,16 +2676,19 @@
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="2"/>
-        <v>5371</v>
+        <v>6958</v>
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="3"/>
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="S16" t="s">
         <v>38</v>
       </c>
       <c r="T16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z16" t="s">
         <v>38</v>
       </c>
       <c r="AA16" s="2" t="s">
@@ -2609,7 +2699,7 @@
       </c>
       <c r="AC16">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD16">
         <v>1</v>
@@ -2624,7 +2714,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
@@ -2654,6 +2744,9 @@
       <c r="M17" t="s">
         <v>333</v>
       </c>
+      <c r="N17" t="s">
+        <v>38</v>
+      </c>
       <c r="O17" t="s">
         <v>349</v>
       </c>
@@ -2662,16 +2755,19 @@
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="2"/>
-        <v>2999</v>
+        <v>3949</v>
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="3"/>
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="S17" t="s">
         <v>38</v>
       </c>
       <c r="T17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z17" t="s">
         <v>38</v>
       </c>
       <c r="AA17" s="2" t="s">
@@ -2697,7 +2793,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
@@ -2727,6 +2823,9 @@
       <c r="M18" t="s">
         <v>334</v>
       </c>
+      <c r="N18" t="s">
+        <v>38</v>
+      </c>
       <c r="O18" t="s">
         <v>318</v>
       </c>
@@ -2735,16 +2834,19 @@
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="2"/>
-        <v>8907</v>
+        <v>9652</v>
       </c>
       <c r="R18">
         <f t="shared" ca="1" si="3"/>
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="S18" t="s">
         <v>38</v>
       </c>
       <c r="T18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z18" t="s">
         <v>38</v>
       </c>
       <c r="AA18" s="2" t="s">
@@ -2755,7 +2857,7 @@
       </c>
       <c r="AC18">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD18">
         <v>1</v>
@@ -2770,11 +2872,11 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" t="s">
         <v>56</v>
@@ -2800,6 +2902,9 @@
       <c r="M19" t="s">
         <v>335</v>
       </c>
+      <c r="N19" t="s">
+        <v>38</v>
+      </c>
       <c r="O19" t="s">
         <v>319</v>
       </c>
@@ -2808,16 +2913,19 @@
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="2"/>
-        <v>6965</v>
+        <v>881</v>
       </c>
       <c r="R19">
         <f t="shared" ca="1" si="3"/>
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="S19" t="s">
         <v>38</v>
       </c>
       <c r="T19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z19" t="s">
         <v>38</v>
       </c>
       <c r="AA19" s="2" t="s">
@@ -2843,11 +2951,11 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
         <v>57</v>
@@ -2873,6 +2981,9 @@
       <c r="M20" t="s">
         <v>336</v>
       </c>
+      <c r="N20" t="s">
+        <v>38</v>
+      </c>
       <c r="O20" t="s">
         <v>320</v>
       </c>
@@ -2881,16 +2992,19 @@
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="2"/>
-        <v>8469</v>
+        <v>9806</v>
       </c>
       <c r="R20">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="S20" t="s">
         <v>38</v>
       </c>
       <c r="T20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z20" t="s">
         <v>38</v>
       </c>
       <c r="AA20" s="2" t="s">
@@ -2901,7 +3015,7 @@
       </c>
       <c r="AC20">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD20">
         <v>1</v>
@@ -2916,7 +3030,7 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
@@ -2946,6 +3060,9 @@
       <c r="M21" t="s">
         <v>337</v>
       </c>
+      <c r="N21" t="s">
+        <v>38</v>
+      </c>
       <c r="O21" t="s">
         <v>321</v>
       </c>
@@ -2954,16 +3071,19 @@
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="2"/>
-        <v>8655</v>
+        <v>870</v>
       </c>
       <c r="R21">
         <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="S21" t="s">
         <v>38</v>
       </c>
       <c r="T21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z21" t="s">
         <v>38</v>
       </c>
       <c r="AA21" s="2" t="s">
@@ -2989,11 +3109,11 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E22" t="s">
         <v>59</v>
@@ -3019,6 +3139,9 @@
       <c r="M22" t="s">
         <v>338</v>
       </c>
+      <c r="N22" t="s">
+        <v>38</v>
+      </c>
       <c r="O22" t="s">
         <v>322</v>
       </c>
@@ -3027,16 +3150,19 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="2"/>
-        <v>3500</v>
+        <v>3372</v>
       </c>
       <c r="R22">
         <f t="shared" ca="1" si="3"/>
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="S22" t="s">
         <v>38</v>
       </c>
       <c r="T22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z22" t="s">
         <v>38</v>
       </c>
       <c r="AA22" s="2" t="s">
@@ -3047,7 +3173,7 @@
       </c>
       <c r="AC22">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD22">
         <v>1</v>
@@ -3066,7 +3192,7 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
         <v>60</v>
@@ -3092,6 +3218,9 @@
       <c r="M23" t="s">
         <v>339</v>
       </c>
+      <c r="N23" t="s">
+        <v>38</v>
+      </c>
       <c r="O23" t="s">
         <v>323</v>
       </c>
@@ -3100,16 +3229,19 @@
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="2"/>
-        <v>2308</v>
+        <v>6380</v>
       </c>
       <c r="R23">
         <f t="shared" ca="1" si="3"/>
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="S23" t="s">
         <v>38</v>
       </c>
       <c r="T23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z23" t="s">
         <v>38</v>
       </c>
       <c r="AA23" s="2" t="s">
@@ -3135,11 +3267,11 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
         <v>61</v>
@@ -3165,6 +3297,9 @@
       <c r="M24" t="s">
         <v>340</v>
       </c>
+      <c r="N24" t="s">
+        <v>38</v>
+      </c>
       <c r="O24" t="s">
         <v>324</v>
       </c>
@@ -3173,16 +3308,19 @@
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="2"/>
-        <v>461</v>
+        <v>6432</v>
       </c>
       <c r="R24">
         <f t="shared" ca="1" si="3"/>
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="S24" t="s">
         <v>38</v>
       </c>
       <c r="T24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z24" t="s">
         <v>38</v>
       </c>
       <c r="AA24" s="2" t="s">
@@ -3208,7 +3346,7 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
@@ -3238,6 +3376,9 @@
       <c r="M25" t="s">
         <v>341</v>
       </c>
+      <c r="N25" t="s">
+        <v>38</v>
+      </c>
       <c r="O25" t="s">
         <v>325</v>
       </c>
@@ -3246,16 +3387,19 @@
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="2"/>
-        <v>9073</v>
+        <v>1477</v>
       </c>
       <c r="R25">
         <f t="shared" ca="1" si="3"/>
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="S25" t="s">
         <v>38</v>
       </c>
       <c r="T25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z25" t="s">
         <v>38</v>
       </c>
       <c r="AA25" s="2" t="s">
@@ -3266,7 +3410,7 @@
       </c>
       <c r="AC25">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD25">
         <v>1</v>
@@ -3281,11 +3425,11 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E26" t="s">
         <v>63</v>
@@ -3311,6 +3455,9 @@
       <c r="M26" t="s">
         <v>342</v>
       </c>
+      <c r="N26" t="s">
+        <v>38</v>
+      </c>
       <c r="O26" t="s">
         <v>326</v>
       </c>
@@ -3319,16 +3466,19 @@
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="2"/>
-        <v>307</v>
+        <v>2139</v>
       </c>
       <c r="R26">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="S26" t="s">
         <v>38</v>
       </c>
       <c r="T26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z26" t="s">
         <v>38</v>
       </c>
       <c r="AA26" s="2" t="s">
@@ -3354,11 +3504,11 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E27" t="s">
         <v>64</v>
@@ -3384,6 +3534,9 @@
       <c r="M27" t="s">
         <v>343</v>
       </c>
+      <c r="N27" t="s">
+        <v>38</v>
+      </c>
       <c r="O27" t="s">
         <v>327</v>
       </c>
@@ -3392,16 +3545,19 @@
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="2"/>
-        <v>896</v>
+        <v>8341</v>
       </c>
       <c r="R27">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="S27" t="s">
         <v>38</v>
       </c>
       <c r="T27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z27" t="s">
         <v>38</v>
       </c>
       <c r="AA27" s="2" t="s">
@@ -3427,11 +3583,11 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
         <v>65</v>
@@ -3457,6 +3613,9 @@
       <c r="M28" t="s">
         <v>344</v>
       </c>
+      <c r="N28" t="s">
+        <v>38</v>
+      </c>
       <c r="O28" t="s">
         <v>328</v>
       </c>
@@ -3465,16 +3624,19 @@
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="2"/>
-        <v>6671</v>
+        <v>5568</v>
       </c>
       <c r="R28">
         <f t="shared" ca="1" si="3"/>
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="S28" t="s">
         <v>38</v>
       </c>
       <c r="T28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z28" t="s">
         <v>38</v>
       </c>
       <c r="AA28" s="2" t="s">
@@ -3485,7 +3647,7 @@
       </c>
       <c r="AC28">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD28">
         <v>1</v>
@@ -3500,11 +3662,11 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E29" t="s">
         <v>66</v>
@@ -3530,6 +3692,9 @@
       <c r="M29" t="s">
         <v>345</v>
       </c>
+      <c r="N29" t="s">
+        <v>38</v>
+      </c>
       <c r="O29" t="s">
         <v>329</v>
       </c>
@@ -3538,16 +3703,19 @@
       </c>
       <c r="Q29">
         <f t="shared" ca="1" si="2"/>
-        <v>3445</v>
+        <v>3601</v>
       </c>
       <c r="R29">
         <f t="shared" ca="1" si="3"/>
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="S29" t="s">
         <v>38</v>
       </c>
       <c r="T29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z29" t="s">
         <v>38</v>
       </c>
       <c r="AA29" s="2" t="s">
@@ -3558,7 +3726,7 @@
       </c>
       <c r="AC29">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD29">
         <v>1</v>
@@ -3577,7 +3745,7 @@
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
         <v>67</v>
@@ -3603,6 +3771,9 @@
       <c r="M30" t="s">
         <v>346</v>
       </c>
+      <c r="N30" t="s">
+        <v>38</v>
+      </c>
       <c r="O30" t="s">
         <v>330</v>
       </c>
@@ -3611,16 +3782,19 @@
       </c>
       <c r="Q30">
         <f t="shared" ca="1" si="2"/>
-        <v>6443</v>
+        <v>2314</v>
       </c>
       <c r="R30">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>152</v>
       </c>
       <c r="S30" t="s">
         <v>38</v>
       </c>
       <c r="T30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z30" t="s">
         <v>38</v>
       </c>
       <c r="AA30" s="2" t="s">
@@ -3646,7 +3820,7 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="1"/>
@@ -3673,6 +3847,9 @@
       <c r="M31" t="s">
         <v>347</v>
       </c>
+      <c r="N31" t="s">
+        <v>38</v>
+      </c>
       <c r="O31" t="s">
         <v>331</v>
       </c>
@@ -3681,16 +3858,19 @@
       </c>
       <c r="Q31">
         <f t="shared" ca="1" si="2"/>
-        <v>9297</v>
+        <v>235</v>
       </c>
       <c r="R31">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="S31" t="s">
         <v>38</v>
       </c>
       <c r="T31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z31" t="s">
         <v>38</v>
       </c>
       <c r="AA31" s="2" t="s">
@@ -3716,7 +3896,7 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="1"/>
@@ -3743,6 +3923,9 @@
       <c r="M32" t="s">
         <v>348</v>
       </c>
+      <c r="N32" t="s">
+        <v>38</v>
+      </c>
       <c r="O32" t="s">
         <v>332</v>
       </c>
@@ -3751,16 +3934,19 @@
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="2"/>
-        <v>890</v>
+        <v>849</v>
       </c>
       <c r="R32">
         <f t="shared" ca="1" si="3"/>
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="S32" t="s">
         <v>38</v>
       </c>
       <c r="T32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z32" t="s">
         <v>38</v>
       </c>
       <c r="AA32" s="2" t="s">
@@ -3790,7 +3976,7 @@
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E33" t="s">
         <v>70</v>
@@ -3813,6 +3999,9 @@
       <c r="M33" t="s">
         <v>349</v>
       </c>
+      <c r="N33" t="s">
+        <v>38</v>
+      </c>
       <c r="O33" t="s">
         <v>333</v>
       </c>
@@ -3821,11 +4010,11 @@
       </c>
       <c r="Q33">
         <f t="shared" ca="1" si="2"/>
-        <v>2044</v>
+        <v>8533</v>
       </c>
       <c r="R33">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="S33" t="s">
         <v>38</v>
@@ -3833,6 +4022,9 @@
       <c r="T33" s="1">
         <v>16552688</v>
       </c>
+      <c r="Z33" t="s">
+        <v>38</v>
+      </c>
       <c r="AA33" s="2" t="s">
         <v>38</v>
       </c>
@@ -3841,7 +4033,7 @@
       </c>
       <c r="AC33">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD33">
         <v>1</v>
@@ -3856,11 +4048,11 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
         <v>71</v>
@@ -3883,6 +4075,9 @@
       <c r="M34" t="s">
         <v>318</v>
       </c>
+      <c r="N34" t="s">
+        <v>38</v>
+      </c>
       <c r="O34" t="s">
         <v>334</v>
       </c>
@@ -3891,16 +4086,19 @@
       </c>
       <c r="Q34">
         <f t="shared" ca="1" si="2"/>
-        <v>5212</v>
+        <v>1739</v>
       </c>
       <c r="R34">
         <f t="shared" ca="1" si="3"/>
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="S34" t="s">
         <v>38</v>
       </c>
       <c r="T34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z34" t="s">
         <v>38</v>
       </c>
       <c r="AA34" s="2" t="s">
@@ -3926,11 +4124,11 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E35" t="s">
         <v>72</v>
@@ -3953,6 +4151,9 @@
       <c r="M35" t="s">
         <v>319</v>
       </c>
+      <c r="N35" t="s">
+        <v>38</v>
+      </c>
       <c r="O35" t="s">
         <v>335</v>
       </c>
@@ -3961,16 +4162,19 @@
       </c>
       <c r="Q35">
         <f t="shared" ca="1" si="2"/>
-        <v>2126</v>
+        <v>6452</v>
       </c>
       <c r="R35">
         <f t="shared" ca="1" si="3"/>
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="S35" t="s">
         <v>38</v>
       </c>
       <c r="T35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z35" t="s">
         <v>38</v>
       </c>
       <c r="AA35" s="2" t="s">
@@ -3996,7 +4200,7 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="1"/>
@@ -4023,6 +4227,9 @@
       <c r="M36" t="s">
         <v>320</v>
       </c>
+      <c r="N36" t="s">
+        <v>38</v>
+      </c>
       <c r="O36" t="s">
         <v>336</v>
       </c>
@@ -4031,16 +4238,19 @@
       </c>
       <c r="Q36">
         <f t="shared" ca="1" si="2"/>
-        <v>9197</v>
+        <v>5427</v>
       </c>
       <c r="R36">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="S36" t="s">
         <v>38</v>
       </c>
       <c r="T36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z36" t="s">
         <v>38</v>
       </c>
       <c r="AA36" s="2" t="s">
@@ -4066,11 +4276,11 @@
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37" t="s">
         <v>74</v>
@@ -4093,6 +4303,9 @@
       <c r="M37" t="s">
         <v>321</v>
       </c>
+      <c r="N37" t="s">
+        <v>38</v>
+      </c>
       <c r="O37" t="s">
         <v>337</v>
       </c>
@@ -4101,16 +4314,19 @@
       </c>
       <c r="Q37">
         <f t="shared" ca="1" si="2"/>
-        <v>917</v>
+        <v>1444</v>
       </c>
       <c r="R37">
         <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="S37" t="s">
         <v>38</v>
       </c>
       <c r="T37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z37" t="s">
         <v>38</v>
       </c>
       <c r="AA37" s="2" t="s">
@@ -4121,7 +4337,7 @@
       </c>
       <c r="AC37">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD37">
         <v>1</v>
@@ -4136,11 +4352,11 @@
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
         <v>75</v>
@@ -4163,6 +4379,9 @@
       <c r="M38" t="s">
         <v>322</v>
       </c>
+      <c r="N38" t="s">
+        <v>38</v>
+      </c>
       <c r="O38" t="s">
         <v>338</v>
       </c>
@@ -4171,16 +4390,19 @@
       </c>
       <c r="Q38">
         <f t="shared" ca="1" si="2"/>
-        <v>4072</v>
+        <v>3339</v>
       </c>
       <c r="R38">
         <f t="shared" ca="1" si="3"/>
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="S38" t="s">
         <v>38</v>
       </c>
       <c r="T38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z38" t="s">
         <v>38</v>
       </c>
       <c r="AA38" s="2" t="s">
@@ -4206,11 +4428,11 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E39" t="s">
         <v>76</v>
@@ -4233,6 +4455,9 @@
       <c r="M39" t="s">
         <v>323</v>
       </c>
+      <c r="N39" t="s">
+        <v>38</v>
+      </c>
       <c r="O39" t="s">
         <v>339</v>
       </c>
@@ -4241,16 +4466,19 @@
       </c>
       <c r="Q39">
         <f t="shared" ca="1" si="2"/>
-        <v>7373</v>
+        <v>6250</v>
       </c>
       <c r="R39">
         <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="S39" t="s">
         <v>38</v>
       </c>
       <c r="T39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z39" t="s">
         <v>38</v>
       </c>
       <c r="AA39" s="2" t="s">
@@ -4276,7 +4504,7 @@
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="1"/>
@@ -4303,6 +4531,9 @@
       <c r="M40" t="s">
         <v>324</v>
       </c>
+      <c r="N40" t="s">
+        <v>38</v>
+      </c>
       <c r="O40" t="s">
         <v>340</v>
       </c>
@@ -4311,16 +4542,19 @@
       </c>
       <c r="Q40">
         <f t="shared" ca="1" si="2"/>
-        <v>8197</v>
+        <v>6738</v>
       </c>
       <c r="R40">
         <f t="shared" ca="1" si="3"/>
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="S40" t="s">
         <v>38</v>
       </c>
       <c r="T40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z40" t="s">
         <v>38</v>
       </c>
       <c r="AA40" s="2" t="s">
@@ -4346,11 +4580,11 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E41" t="s">
         <v>77</v>
@@ -4373,6 +4607,9 @@
       <c r="M41" t="s">
         <v>325</v>
       </c>
+      <c r="N41" t="s">
+        <v>38</v>
+      </c>
       <c r="O41" t="s">
         <v>341</v>
       </c>
@@ -4381,16 +4618,19 @@
       </c>
       <c r="Q41">
         <f t="shared" ca="1" si="2"/>
-        <v>228</v>
+        <v>3983</v>
       </c>
       <c r="R41">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="S41" t="s">
         <v>38</v>
       </c>
       <c r="T41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z41" t="s">
         <v>38</v>
       </c>
       <c r="AA41" s="2" t="s">
@@ -4420,7 +4660,7 @@
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E42" t="s">
         <v>78</v>
@@ -4443,6 +4683,9 @@
       <c r="M42" t="s">
         <v>326</v>
       </c>
+      <c r="N42" t="s">
+        <v>38</v>
+      </c>
       <c r="O42" t="s">
         <v>342</v>
       </c>
@@ -4451,16 +4694,19 @@
       </c>
       <c r="Q42">
         <f t="shared" ca="1" si="2"/>
-        <v>9512</v>
+        <v>7630</v>
       </c>
       <c r="R42">
         <f t="shared" ca="1" si="3"/>
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="S42" t="s">
         <v>38</v>
       </c>
       <c r="T42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z42" t="s">
         <v>38</v>
       </c>
       <c r="AA42" s="2" t="s">
@@ -4486,7 +4732,7 @@
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="1"/>
@@ -4513,6 +4759,9 @@
       <c r="M43" t="s">
         <v>327</v>
       </c>
+      <c r="N43" t="s">
+        <v>38</v>
+      </c>
       <c r="O43" t="s">
         <v>343</v>
       </c>
@@ -4521,16 +4770,19 @@
       </c>
       <c r="Q43">
         <f t="shared" ca="1" si="2"/>
-        <v>8434</v>
+        <v>449</v>
       </c>
       <c r="R43">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="S43" t="s">
         <v>38</v>
       </c>
       <c r="T43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z43" t="s">
         <v>38</v>
       </c>
       <c r="AA43" s="2" t="s">
@@ -4556,7 +4808,7 @@
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="1"/>
@@ -4583,6 +4835,9 @@
       <c r="M44" t="s">
         <v>328</v>
       </c>
+      <c r="N44" t="s">
+        <v>38</v>
+      </c>
       <c r="O44" t="s">
         <v>344</v>
       </c>
@@ -4591,16 +4846,19 @@
       </c>
       <c r="Q44">
         <f t="shared" ca="1" si="2"/>
-        <v>1446</v>
+        <v>9137</v>
       </c>
       <c r="R44">
         <f t="shared" ca="1" si="3"/>
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="S44" t="s">
         <v>38</v>
       </c>
       <c r="T44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z44" t="s">
         <v>38</v>
       </c>
       <c r="AA44" s="2" t="s">
@@ -4611,7 +4869,7 @@
       </c>
       <c r="AC44">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD44">
         <v>1</v>
@@ -4626,11 +4884,11 @@
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E45" t="s">
         <v>81</v>
@@ -4653,6 +4911,9 @@
       <c r="M45" t="s">
         <v>329</v>
       </c>
+      <c r="N45" t="s">
+        <v>38</v>
+      </c>
       <c r="O45" t="s">
         <v>345</v>
       </c>
@@ -4661,16 +4922,19 @@
       </c>
       <c r="Q45">
         <f t="shared" ca="1" si="2"/>
-        <v>2686</v>
+        <v>2110</v>
       </c>
       <c r="R45">
         <f t="shared" ca="1" si="3"/>
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="S45" t="s">
         <v>38</v>
       </c>
       <c r="T45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z45" t="s">
         <v>38</v>
       </c>
       <c r="AA45" s="2" t="s">
@@ -4696,11 +4960,11 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E46" t="s">
         <v>82</v>
@@ -4723,6 +4987,9 @@
       <c r="M46" t="s">
         <v>330</v>
       </c>
+      <c r="N46" t="s">
+        <v>38</v>
+      </c>
       <c r="O46" t="s">
         <v>346</v>
       </c>
@@ -4731,16 +4998,19 @@
       </c>
       <c r="Q46">
         <f t="shared" ca="1" si="2"/>
-        <v>8980</v>
+        <v>5299</v>
       </c>
       <c r="R46">
         <f t="shared" ca="1" si="3"/>
-        <v>146</v>
+        <v>39</v>
       </c>
       <c r="S46" t="s">
         <v>38</v>
       </c>
       <c r="T46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z46" t="s">
         <v>38</v>
       </c>
       <c r="AA46" s="2" t="s">
@@ -4770,7 +5040,7 @@
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E47" t="s">
         <v>83</v>
@@ -4793,6 +5063,9 @@
       <c r="M47" t="s">
         <v>331</v>
       </c>
+      <c r="N47" t="s">
+        <v>38</v>
+      </c>
       <c r="O47" t="s">
         <v>347</v>
       </c>
@@ -4801,16 +5074,19 @@
       </c>
       <c r="Q47">
         <f t="shared" ca="1" si="2"/>
-        <v>1223</v>
+        <v>7512</v>
       </c>
       <c r="R47">
         <f t="shared" ca="1" si="3"/>
-        <v>129</v>
+        <v>13</v>
       </c>
       <c r="S47" t="s">
         <v>38</v>
       </c>
       <c r="T47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z47" t="s">
         <v>38</v>
       </c>
       <c r="AA47" s="2" t="s">
@@ -4821,7 +5097,7 @@
       </c>
       <c r="AC47">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD47">
         <v>1</v>
@@ -4836,11 +5112,11 @@
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
         <v>84</v>
@@ -4863,6 +5139,9 @@
       <c r="M48" t="s">
         <v>332</v>
       </c>
+      <c r="N48" t="s">
+        <v>38</v>
+      </c>
       <c r="O48" t="s">
         <v>348</v>
       </c>
@@ -4871,16 +5150,19 @@
       </c>
       <c r="Q48">
         <f t="shared" ca="1" si="2"/>
-        <v>9270</v>
+        <v>1288</v>
       </c>
       <c r="R48">
         <f t="shared" ca="1" si="3"/>
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="S48" t="s">
         <v>38</v>
       </c>
       <c r="T48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z48" t="s">
         <v>38</v>
       </c>
       <c r="AA48" s="2" t="s">
@@ -4933,6 +5215,9 @@
       <c r="M49" t="s">
         <v>333</v>
       </c>
+      <c r="N49" t="s">
+        <v>38</v>
+      </c>
       <c r="O49" t="s">
         <v>349</v>
       </c>
@@ -4941,16 +5226,19 @@
       </c>
       <c r="Q49">
         <f t="shared" ca="1" si="2"/>
-        <v>5652</v>
+        <v>5859</v>
       </c>
       <c r="R49">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="S49" t="s">
         <v>38</v>
       </c>
       <c r="T49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z49" t="s">
         <v>38</v>
       </c>
       <c r="AA49" s="2" t="s">
@@ -4961,7 +5249,7 @@
       </c>
       <c r="AC49">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD49">
         <v>1</v>
@@ -4976,7 +5264,7 @@
       </c>
       <c r="C50">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="1"/>
@@ -5003,6 +5291,9 @@
       <c r="M50" t="s">
         <v>334</v>
       </c>
+      <c r="N50" t="s">
+        <v>38</v>
+      </c>
       <c r="O50" t="s">
         <v>318</v>
       </c>
@@ -5011,16 +5302,19 @@
       </c>
       <c r="Q50">
         <f t="shared" ca="1" si="2"/>
-        <v>1915</v>
+        <v>3083</v>
       </c>
       <c r="R50">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="S50" t="s">
         <v>38</v>
       </c>
       <c r="T50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z50" t="s">
         <v>38</v>
       </c>
       <c r="AA50" s="2" t="s">
@@ -5031,7 +5325,7 @@
       </c>
       <c r="AC50">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD50">
         <v>1</v>
@@ -5046,11 +5340,11 @@
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" t="s">
         <v>87</v>
@@ -5073,6 +5367,9 @@
       <c r="M51" t="s">
         <v>335</v>
       </c>
+      <c r="N51" t="s">
+        <v>38</v>
+      </c>
       <c r="O51" t="s">
         <v>319</v>
       </c>
@@ -5081,16 +5378,19 @@
       </c>
       <c r="Q51">
         <f t="shared" ca="1" si="2"/>
-        <v>4784</v>
+        <v>8783</v>
       </c>
       <c r="R51">
         <f t="shared" ca="1" si="3"/>
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="S51" t="s">
         <v>38</v>
       </c>
       <c r="T51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z51" t="s">
         <v>38</v>
       </c>
       <c r="AA51" s="2" t="s">
@@ -5101,7 +5401,7 @@
       </c>
       <c r="AC51">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD51">
         <v>1</v>
@@ -5116,11 +5416,11 @@
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E52" t="s">
         <v>88</v>
@@ -5143,6 +5443,9 @@
       <c r="M52" t="s">
         <v>336</v>
       </c>
+      <c r="N52" t="s">
+        <v>38</v>
+      </c>
       <c r="O52" t="s">
         <v>320</v>
       </c>
@@ -5151,16 +5454,19 @@
       </c>
       <c r="Q52">
         <f t="shared" ca="1" si="2"/>
-        <v>8945</v>
+        <v>4090</v>
       </c>
       <c r="R52">
         <f t="shared" ca="1" si="3"/>
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="S52" t="s">
         <v>38</v>
       </c>
       <c r="T52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z52" t="s">
         <v>38</v>
       </c>
       <c r="AA52" s="2" t="s">
@@ -5213,6 +5519,9 @@
       <c r="M53" t="s">
         <v>337</v>
       </c>
+      <c r="N53" t="s">
+        <v>38</v>
+      </c>
       <c r="O53" t="s">
         <v>321</v>
       </c>
@@ -5221,16 +5530,19 @@
       </c>
       <c r="Q53">
         <f t="shared" ca="1" si="2"/>
-        <v>8547</v>
+        <v>462</v>
       </c>
       <c r="R53">
         <f t="shared" ca="1" si="3"/>
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="S53" t="s">
         <v>38</v>
       </c>
       <c r="T53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z53" t="s">
         <v>38</v>
       </c>
       <c r="AA53" s="2" t="s">
@@ -5256,11 +5568,11 @@
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E54" t="s">
         <v>90</v>
@@ -5283,6 +5595,9 @@
       <c r="M54" t="s">
         <v>338</v>
       </c>
+      <c r="N54" t="s">
+        <v>38</v>
+      </c>
       <c r="O54" t="s">
         <v>322</v>
       </c>
@@ -5291,16 +5606,19 @@
       </c>
       <c r="Q54">
         <f t="shared" ca="1" si="2"/>
-        <v>6515</v>
+        <v>4040</v>
       </c>
       <c r="R54">
         <f t="shared" ca="1" si="3"/>
-        <v>136</v>
+        <v>34</v>
       </c>
       <c r="S54" t="s">
         <v>38</v>
       </c>
       <c r="T54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z54" t="s">
         <v>38</v>
       </c>
       <c r="AA54" s="2" t="s">
@@ -5311,7 +5629,7 @@
       </c>
       <c r="AC54">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD54">
         <v>1</v>
@@ -5326,11 +5644,11 @@
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E55" t="s">
         <v>91</v>
@@ -5353,6 +5671,9 @@
       <c r="M55" t="s">
         <v>339</v>
       </c>
+      <c r="N55" t="s">
+        <v>38</v>
+      </c>
       <c r="O55" t="s">
         <v>323</v>
       </c>
@@ -5361,16 +5682,19 @@
       </c>
       <c r="Q55">
         <f t="shared" ca="1" si="2"/>
-        <v>5463</v>
+        <v>6051</v>
       </c>
       <c r="R55">
         <f t="shared" ca="1" si="3"/>
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="S55" t="s">
         <v>38</v>
       </c>
       <c r="T55" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z55" t="s">
         <v>38</v>
       </c>
       <c r="AA55" s="2" t="s">
@@ -5396,11 +5720,11 @@
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E56" t="s">
         <v>92</v>
@@ -5423,6 +5747,9 @@
       <c r="M56" t="s">
         <v>340</v>
       </c>
+      <c r="N56" t="s">
+        <v>38</v>
+      </c>
       <c r="O56" t="s">
         <v>324</v>
       </c>
@@ -5431,16 +5758,19 @@
       </c>
       <c r="Q56">
         <f t="shared" ca="1" si="2"/>
-        <v>2409</v>
+        <v>5897</v>
       </c>
       <c r="R56">
         <f t="shared" ca="1" si="3"/>
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="S56" t="s">
         <v>38</v>
       </c>
       <c r="T56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z56" t="s">
         <v>38</v>
       </c>
       <c r="AA56" s="2" t="s">
@@ -5451,7 +5781,7 @@
       </c>
       <c r="AC56">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD56">
         <v>1</v>
@@ -5466,11 +5796,11 @@
       </c>
       <c r="C57">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E57" t="s">
         <v>93</v>
@@ -5493,6 +5823,9 @@
       <c r="M57" t="s">
         <v>341</v>
       </c>
+      <c r="N57" t="s">
+        <v>38</v>
+      </c>
       <c r="O57" t="s">
         <v>325</v>
       </c>
@@ -5501,16 +5834,19 @@
       </c>
       <c r="Q57">
         <f t="shared" ca="1" si="2"/>
-        <v>8219</v>
+        <v>4968</v>
       </c>
       <c r="R57">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="S57" t="s">
         <v>38</v>
       </c>
       <c r="T57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z57" t="s">
         <v>38</v>
       </c>
       <c r="AA57" s="2">
@@ -5536,11 +5872,11 @@
       </c>
       <c r="C58">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E58" t="s">
         <v>94</v>
@@ -5563,6 +5899,9 @@
       <c r="M58" t="s">
         <v>342</v>
       </c>
+      <c r="N58" t="s">
+        <v>38</v>
+      </c>
       <c r="O58" t="s">
         <v>326</v>
       </c>
@@ -5571,16 +5910,19 @@
       </c>
       <c r="Q58">
         <f t="shared" ca="1" si="2"/>
-        <v>4472</v>
+        <v>1474</v>
       </c>
       <c r="R58">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="S58" t="s">
         <v>38</v>
       </c>
       <c r="T58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z58" t="s">
         <v>38</v>
       </c>
       <c r="AA58" s="2" t="s">
@@ -5606,7 +5948,7 @@
       </c>
       <c r="C59">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="1"/>
@@ -5633,6 +5975,9 @@
       <c r="M59" t="s">
         <v>343</v>
       </c>
+      <c r="N59" t="s">
+        <v>38</v>
+      </c>
       <c r="O59" t="s">
         <v>327</v>
       </c>
@@ -5641,16 +5986,19 @@
       </c>
       <c r="Q59">
         <f t="shared" ca="1" si="2"/>
-        <v>2211</v>
+        <v>1723</v>
       </c>
       <c r="R59">
         <f t="shared" ca="1" si="3"/>
-        <v>127</v>
+        <v>71</v>
       </c>
       <c r="S59" t="s">
         <v>38</v>
       </c>
       <c r="T59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z59" t="s">
         <v>38</v>
       </c>
       <c r="AA59" s="2" t="s">
@@ -5676,11 +6024,11 @@
       </c>
       <c r="C60">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E60" t="s">
         <v>96</v>
@@ -5703,6 +6051,9 @@
       <c r="M60" t="s">
         <v>344</v>
       </c>
+      <c r="N60" t="s">
+        <v>38</v>
+      </c>
       <c r="O60" t="s">
         <v>328</v>
       </c>
@@ -5711,16 +6062,19 @@
       </c>
       <c r="Q60">
         <f t="shared" ca="1" si="2"/>
-        <v>9421</v>
+        <v>874</v>
       </c>
       <c r="R60">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="S60" t="s">
         <v>38</v>
       </c>
       <c r="T60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z60" t="s">
         <v>38</v>
       </c>
       <c r="AA60" s="2" t="s">
@@ -5731,7 +6085,7 @@
       </c>
       <c r="AC60">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD60">
         <v>1</v>
@@ -5746,11 +6100,11 @@
       </c>
       <c r="C61">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E61" t="s">
         <v>97</v>
@@ -5773,6 +6127,9 @@
       <c r="M61" t="s">
         <v>345</v>
       </c>
+      <c r="N61" t="s">
+        <v>38</v>
+      </c>
       <c r="O61" t="s">
         <v>329</v>
       </c>
@@ -5781,16 +6138,19 @@
       </c>
       <c r="Q61">
         <f t="shared" ca="1" si="2"/>
-        <v>8493</v>
+        <v>652</v>
       </c>
       <c r="R61">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="S61" t="s">
         <v>38</v>
       </c>
       <c r="T61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z61" t="s">
         <v>38</v>
       </c>
       <c r="AA61" s="2" t="s">
@@ -5801,7 +6161,7 @@
       </c>
       <c r="AC61">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD61">
         <v>1</v>
@@ -5816,11 +6176,11 @@
       </c>
       <c r="C62">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E62" t="s">
         <v>98</v>
@@ -5843,6 +6203,9 @@
       <c r="M62" t="s">
         <v>346</v>
       </c>
+      <c r="N62" t="s">
+        <v>38</v>
+      </c>
       <c r="O62" t="s">
         <v>330</v>
       </c>
@@ -5851,16 +6214,19 @@
       </c>
       <c r="Q62">
         <f t="shared" ca="1" si="2"/>
-        <v>3292</v>
+        <v>5101</v>
       </c>
       <c r="R62">
         <f t="shared" ca="1" si="3"/>
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="S62" t="s">
         <v>38</v>
       </c>
       <c r="T62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z62" t="s">
         <v>38</v>
       </c>
       <c r="AA62" s="2" t="s">
@@ -5886,11 +6252,11 @@
       </c>
       <c r="C63">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E63" t="s">
         <v>99</v>
@@ -5913,6 +6279,9 @@
       <c r="M63" t="s">
         <v>347</v>
       </c>
+      <c r="N63" t="s">
+        <v>38</v>
+      </c>
       <c r="O63" t="s">
         <v>331</v>
       </c>
@@ -5921,16 +6290,19 @@
       </c>
       <c r="Q63">
         <f t="shared" ca="1" si="2"/>
-        <v>4875</v>
+        <v>8339</v>
       </c>
       <c r="R63">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="S63" t="s">
         <v>38</v>
       </c>
       <c r="T63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z63" t="s">
         <v>38</v>
       </c>
       <c r="AA63" s="2" t="s">
@@ -5941,7 +6313,7 @@
       </c>
       <c r="AC63">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD63">
         <v>1</v>
@@ -5956,11 +6328,11 @@
       </c>
       <c r="C64">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E64" t="s">
         <v>100</v>
@@ -5983,6 +6355,9 @@
       <c r="M64" t="s">
         <v>348</v>
       </c>
+      <c r="N64" t="s">
+        <v>38</v>
+      </c>
       <c r="O64" t="s">
         <v>332</v>
       </c>
@@ -5991,16 +6366,19 @@
       </c>
       <c r="Q64">
         <f t="shared" ca="1" si="2"/>
-        <v>5323</v>
+        <v>865</v>
       </c>
       <c r="R64">
         <f t="shared" ca="1" si="3"/>
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="S64" t="s">
         <v>38</v>
       </c>
       <c r="T64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z64" t="s">
         <v>38</v>
       </c>
       <c r="AA64" s="2" t="s">
@@ -6011,7 +6389,7 @@
       </c>
       <c r="AC64">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD64">
         <v>1</v>
@@ -6026,11 +6404,11 @@
       </c>
       <c r="C65">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E65" t="s">
         <v>101</v>
@@ -6053,6 +6431,9 @@
       <c r="M65" t="s">
         <v>349</v>
       </c>
+      <c r="N65" t="s">
+        <v>38</v>
+      </c>
       <c r="O65" t="s">
         <v>333</v>
       </c>
@@ -6061,7 +6442,7 @@
       </c>
       <c r="Q65">
         <f t="shared" ca="1" si="2"/>
-        <v>894</v>
+        <v>9700</v>
       </c>
       <c r="R65">
         <f t="shared" ca="1" si="3"/>
@@ -6073,6 +6454,9 @@
       <c r="T65" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="Z65" t="s">
+        <v>38</v>
+      </c>
       <c r="AA65" s="2" t="s">
         <v>38</v>
       </c>
@@ -6081,7 +6465,7 @@
       </c>
       <c r="AC65">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD65">
         <v>1</v>
@@ -6096,11 +6480,11 @@
       </c>
       <c r="C66">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E66" t="s">
         <v>102</v>
@@ -6123,6 +6507,9 @@
       <c r="M66" t="s">
         <v>318</v>
       </c>
+      <c r="N66" t="s">
+        <v>38</v>
+      </c>
       <c r="O66" t="s">
         <v>334</v>
       </c>
@@ -6131,16 +6518,19 @@
       </c>
       <c r="Q66">
         <f t="shared" ca="1" si="2"/>
-        <v>5735</v>
+        <v>4519</v>
       </c>
       <c r="R66">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>148</v>
       </c>
       <c r="S66" t="s">
         <v>38</v>
       </c>
       <c r="T66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z66" t="s">
         <v>38</v>
       </c>
       <c r="AA66" s="2" t="s">
@@ -6151,7 +6541,7 @@
       </c>
       <c r="AC66">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD66">
         <v>1</v>
@@ -6166,11 +6556,11 @@
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C101" ca="1" si="5">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D67">
         <f t="shared" ref="D67:D101" ca="1" si="6">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E67" t="s">
         <v>103</v>
@@ -6193,6 +6583,9 @@
       <c r="M67" t="s">
         <v>319</v>
       </c>
+      <c r="N67" t="s">
+        <v>38</v>
+      </c>
       <c r="O67" t="s">
         <v>335</v>
       </c>
@@ -6201,16 +6594,19 @@
       </c>
       <c r="Q67">
         <f t="shared" ref="Q67:Q101" ca="1" si="7">RANDBETWEEN(100,10000)</f>
-        <v>2614</v>
+        <v>4881</v>
       </c>
       <c r="R67">
         <f t="shared" ref="R67:R101" ca="1" si="8">RANDBETWEEN(1,153)</f>
-        <v>152</v>
+        <v>51</v>
       </c>
       <c r="S67" t="s">
         <v>38</v>
       </c>
       <c r="T67" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z67" t="s">
         <v>38</v>
       </c>
       <c r="AA67" s="2" t="s">
@@ -6221,7 +6617,7 @@
       </c>
       <c r="AC67">
         <f t="shared" ref="AC67:AC101" ca="1" si="9">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD67">
         <v>1</v>
@@ -6240,7 +6636,7 @@
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E68" t="s">
         <v>104</v>
@@ -6263,6 +6659,9 @@
       <c r="M68" t="s">
         <v>320</v>
       </c>
+      <c r="N68" t="s">
+        <v>38</v>
+      </c>
       <c r="O68" t="s">
         <v>336</v>
       </c>
@@ -6271,16 +6670,19 @@
       </c>
       <c r="Q68">
         <f t="shared" ca="1" si="7"/>
-        <v>6331</v>
+        <v>8906</v>
       </c>
       <c r="R68">
         <f t="shared" ca="1" si="8"/>
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="S68" t="s">
         <v>38</v>
       </c>
       <c r="T68" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z68" t="s">
         <v>38</v>
       </c>
       <c r="AA68" s="2" t="s">
@@ -6291,7 +6693,7 @@
       </c>
       <c r="AC68">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD68">
         <v>1</v>
@@ -6306,11 +6708,11 @@
       </c>
       <c r="C69">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E69" t="s">
         <v>105</v>
@@ -6333,6 +6735,9 @@
       <c r="M69" t="s">
         <v>321</v>
       </c>
+      <c r="N69" t="s">
+        <v>38</v>
+      </c>
       <c r="O69" t="s">
         <v>337</v>
       </c>
@@ -6341,16 +6746,19 @@
       </c>
       <c r="Q69">
         <f t="shared" ca="1" si="7"/>
-        <v>7973</v>
+        <v>2670</v>
       </c>
       <c r="R69">
         <f t="shared" ca="1" si="8"/>
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="S69" t="s">
         <v>38</v>
       </c>
       <c r="T69" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z69" t="s">
         <v>38</v>
       </c>
       <c r="AA69" s="2" t="s">
@@ -6361,7 +6769,7 @@
       </c>
       <c r="AC69">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD69">
         <v>1</v>
@@ -6376,7 +6784,7 @@
       </c>
       <c r="C70">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="6"/>
@@ -6403,6 +6811,9 @@
       <c r="M70" t="s">
         <v>322</v>
       </c>
+      <c r="N70" t="s">
+        <v>38</v>
+      </c>
       <c r="O70" t="s">
         <v>338</v>
       </c>
@@ -6411,7 +6822,7 @@
       </c>
       <c r="Q70">
         <f t="shared" ca="1" si="7"/>
-        <v>8472</v>
+        <v>9122</v>
       </c>
       <c r="R70">
         <f t="shared" ca="1" si="8"/>
@@ -6423,6 +6834,9 @@
       <c r="T70" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="Z70" t="s">
+        <v>38</v>
+      </c>
       <c r="AA70" s="2" t="s">
         <v>38</v>
       </c>
@@ -6431,7 +6845,7 @@
       </c>
       <c r="AC70">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD70">
         <v>1</v>
@@ -6446,7 +6860,7 @@
       </c>
       <c r="C71">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="6"/>
@@ -6473,6 +6887,9 @@
       <c r="M71" t="s">
         <v>323</v>
       </c>
+      <c r="N71" t="s">
+        <v>38</v>
+      </c>
       <c r="O71" t="s">
         <v>339</v>
       </c>
@@ -6481,16 +6898,19 @@
       </c>
       <c r="Q71">
         <f t="shared" ca="1" si="7"/>
-        <v>4862</v>
+        <v>2955</v>
       </c>
       <c r="R71">
         <f t="shared" ca="1" si="8"/>
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="S71" t="s">
         <v>38</v>
       </c>
       <c r="T71" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z71" t="s">
         <v>38</v>
       </c>
       <c r="AA71" s="2" t="s">
@@ -6520,7 +6940,7 @@
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E72" t="s">
         <v>108</v>
@@ -6543,6 +6963,9 @@
       <c r="M72" t="s">
         <v>324</v>
       </c>
+      <c r="N72" t="s">
+        <v>38</v>
+      </c>
       <c r="O72" t="s">
         <v>340</v>
       </c>
@@ -6551,16 +6974,19 @@
       </c>
       <c r="Q72">
         <f t="shared" ca="1" si="7"/>
-        <v>7092</v>
+        <v>9059</v>
       </c>
       <c r="R72">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="S72" t="s">
         <v>38</v>
       </c>
       <c r="T72" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z72" t="s">
         <v>38</v>
       </c>
       <c r="AA72" s="2" t="s">
@@ -6586,7 +7012,7 @@
       </c>
       <c r="C73">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="6"/>
@@ -6613,6 +7039,9 @@
       <c r="M73" t="s">
         <v>325</v>
       </c>
+      <c r="N73" t="s">
+        <v>38</v>
+      </c>
       <c r="O73" t="s">
         <v>341</v>
       </c>
@@ -6621,17 +7050,20 @@
       </c>
       <c r="Q73">
         <f t="shared" ca="1" si="7"/>
-        <v>9853</v>
+        <v>4124</v>
       </c>
       <c r="R73">
         <f t="shared" ca="1" si="8"/>
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="S73" t="s">
         <v>38</v>
       </c>
       <c r="T73" s="1">
         <v>12246</v>
+      </c>
+      <c r="Z73" t="s">
+        <v>38</v>
       </c>
       <c r="AA73" s="2" t="s">
         <v>317</v>
@@ -6656,11 +7088,11 @@
       </c>
       <c r="C74">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D74">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E74" t="s">
         <v>110</v>
@@ -6683,6 +7115,9 @@
       <c r="M74" t="s">
         <v>326</v>
       </c>
+      <c r="N74" t="s">
+        <v>38</v>
+      </c>
       <c r="O74" t="s">
         <v>342</v>
       </c>
@@ -6691,16 +7126,19 @@
       </c>
       <c r="Q74">
         <f t="shared" ca="1" si="7"/>
-        <v>6793</v>
+        <v>4781</v>
       </c>
       <c r="R74">
         <f t="shared" ca="1" si="8"/>
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="S74" t="s">
         <v>38</v>
       </c>
       <c r="T74" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z74" t="s">
         <v>38</v>
       </c>
       <c r="AA74" s="2" t="s">
@@ -6726,11 +7164,11 @@
       </c>
       <c r="C75">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E75" t="s">
         <v>111</v>
@@ -6750,6 +7188,9 @@
       <c r="M75" t="s">
         <v>327</v>
       </c>
+      <c r="N75" t="s">
+        <v>38</v>
+      </c>
       <c r="O75" t="s">
         <v>343</v>
       </c>
@@ -6758,16 +7199,19 @@
       </c>
       <c r="Q75">
         <f t="shared" ca="1" si="7"/>
-        <v>6350</v>
+        <v>6395</v>
       </c>
       <c r="R75">
         <f t="shared" ca="1" si="8"/>
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="S75" t="s">
         <v>38</v>
       </c>
       <c r="T75" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z75" t="s">
         <v>38</v>
       </c>
       <c r="AA75" s="2" t="s">
@@ -6793,11 +7237,11 @@
       </c>
       <c r="C76">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E76" t="s">
         <v>112</v>
@@ -6817,6 +7261,9 @@
       <c r="M76" t="s">
         <v>328</v>
       </c>
+      <c r="N76" t="s">
+        <v>38</v>
+      </c>
       <c r="O76" t="s">
         <v>344</v>
       </c>
@@ -6825,16 +7272,19 @@
       </c>
       <c r="Q76">
         <f t="shared" ca="1" si="7"/>
-        <v>1411</v>
+        <v>5966</v>
       </c>
       <c r="R76">
         <f t="shared" ca="1" si="8"/>
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="S76" t="s">
         <v>38</v>
       </c>
       <c r="T76" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z76" t="s">
         <v>38</v>
       </c>
       <c r="AA76" s="2" t="s">
@@ -6845,7 +7295,7 @@
       </c>
       <c r="AC76">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD76">
         <v>1</v>
@@ -6860,11 +7310,11 @@
       </c>
       <c r="C77">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E77" t="s">
         <v>113</v>
@@ -6884,6 +7334,9 @@
       <c r="M77" t="s">
         <v>329</v>
       </c>
+      <c r="N77" t="s">
+        <v>38</v>
+      </c>
       <c r="O77" t="s">
         <v>345</v>
       </c>
@@ -6892,16 +7345,19 @@
       </c>
       <c r="Q77">
         <f t="shared" ca="1" si="7"/>
-        <v>9394</v>
+        <v>9509</v>
       </c>
       <c r="R77">
         <f t="shared" ca="1" si="8"/>
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="S77" t="s">
         <v>38</v>
       </c>
       <c r="T77" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z77" t="s">
         <v>38</v>
       </c>
       <c r="AA77" s="2" t="s">
@@ -6927,11 +7383,11 @@
       </c>
       <c r="C78">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E78" t="s">
         <v>114</v>
@@ -6951,6 +7407,9 @@
       <c r="M78" t="s">
         <v>330</v>
       </c>
+      <c r="N78" t="s">
+        <v>38</v>
+      </c>
       <c r="O78" t="s">
         <v>346</v>
       </c>
@@ -6959,16 +7418,19 @@
       </c>
       <c r="Q78">
         <f t="shared" ca="1" si="7"/>
-        <v>1853</v>
+        <v>762</v>
       </c>
       <c r="R78">
         <f t="shared" ca="1" si="8"/>
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="S78" t="s">
         <v>38</v>
       </c>
       <c r="T78" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z78" t="s">
         <v>38</v>
       </c>
       <c r="AA78" s="2" t="s">
@@ -6994,11 +7456,11 @@
       </c>
       <c r="C79">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E79" t="s">
         <v>115</v>
@@ -7018,6 +7480,9 @@
       <c r="M79" t="s">
         <v>331</v>
       </c>
+      <c r="N79" t="s">
+        <v>38</v>
+      </c>
       <c r="O79" t="s">
         <v>347</v>
       </c>
@@ -7026,16 +7491,19 @@
       </c>
       <c r="Q79">
         <f t="shared" ca="1" si="7"/>
-        <v>7567</v>
+        <v>6078</v>
       </c>
       <c r="R79">
         <f t="shared" ca="1" si="8"/>
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="S79" t="s">
         <v>38</v>
       </c>
       <c r="T79" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z79" t="s">
         <v>38</v>
       </c>
       <c r="AA79" s="2" t="s">
@@ -7061,7 +7529,7 @@
       </c>
       <c r="C80">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="6"/>
@@ -7085,6 +7553,9 @@
       <c r="M80" t="s">
         <v>332</v>
       </c>
+      <c r="N80" t="s">
+        <v>38</v>
+      </c>
       <c r="O80" t="s">
         <v>348</v>
       </c>
@@ -7093,16 +7564,19 @@
       </c>
       <c r="Q80">
         <f t="shared" ca="1" si="7"/>
-        <v>9586</v>
+        <v>7319</v>
       </c>
       <c r="R80">
         <f t="shared" ca="1" si="8"/>
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="S80" t="s">
         <v>38</v>
       </c>
       <c r="T80" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z80" t="s">
         <v>38</v>
       </c>
       <c r="AA80" s="2" t="s">
@@ -7128,7 +7602,7 @@
       </c>
       <c r="C81">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D81">
         <f t="shared" ca="1" si="6"/>
@@ -7152,6 +7626,9 @@
       <c r="M81" t="s">
         <v>333</v>
       </c>
+      <c r="N81" t="s">
+        <v>38</v>
+      </c>
       <c r="O81" t="s">
         <v>349</v>
       </c>
@@ -7160,16 +7637,19 @@
       </c>
       <c r="Q81">
         <f t="shared" ca="1" si="7"/>
-        <v>668</v>
+        <v>9788</v>
       </c>
       <c r="R81">
         <f t="shared" ca="1" si="8"/>
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="S81" t="s">
         <v>38</v>
       </c>
       <c r="T81" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z81" t="s">
         <v>38</v>
       </c>
       <c r="AA81" s="2" t="s">
@@ -7180,7 +7660,7 @@
       </c>
       <c r="AC81">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD81">
         <v>1</v>
@@ -7195,11 +7675,11 @@
       </c>
       <c r="C82">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E82" t="s">
         <v>118</v>
@@ -7219,6 +7699,9 @@
       <c r="M82" t="s">
         <v>334</v>
       </c>
+      <c r="N82" t="s">
+        <v>38</v>
+      </c>
       <c r="O82" t="s">
         <v>318</v>
       </c>
@@ -7227,16 +7710,19 @@
       </c>
       <c r="Q82">
         <f t="shared" ca="1" si="7"/>
-        <v>807</v>
+        <v>2272</v>
       </c>
       <c r="R82">
         <f t="shared" ca="1" si="8"/>
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="S82" t="s">
         <v>38</v>
       </c>
       <c r="T82" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z82" t="s">
         <v>38</v>
       </c>
       <c r="AA82" s="2" t="s">
@@ -7262,11 +7748,11 @@
       </c>
       <c r="C83">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E83" t="s">
         <v>119</v>
@@ -7286,6 +7772,9 @@
       <c r="M83" t="s">
         <v>335</v>
       </c>
+      <c r="N83" t="s">
+        <v>38</v>
+      </c>
       <c r="O83" t="s">
         <v>319</v>
       </c>
@@ -7294,16 +7783,19 @@
       </c>
       <c r="Q83">
         <f t="shared" ca="1" si="7"/>
-        <v>9058</v>
+        <v>7723</v>
       </c>
       <c r="R83">
         <f t="shared" ca="1" si="8"/>
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="S83" t="s">
         <v>38</v>
       </c>
       <c r="T83" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z83" t="s">
         <v>38</v>
       </c>
       <c r="AA83" s="2" t="s">
@@ -7314,7 +7806,7 @@
       </c>
       <c r="AC83">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD83">
         <v>1</v>
@@ -7329,11 +7821,11 @@
       </c>
       <c r="C84">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E84" t="s">
         <v>120</v>
@@ -7353,6 +7845,9 @@
       <c r="M84" t="s">
         <v>336</v>
       </c>
+      <c r="N84" t="s">
+        <v>38</v>
+      </c>
       <c r="O84" t="s">
         <v>320</v>
       </c>
@@ -7361,16 +7856,19 @@
       </c>
       <c r="Q84">
         <f t="shared" ca="1" si="7"/>
-        <v>3977</v>
+        <v>5746</v>
       </c>
       <c r="R84">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>145</v>
       </c>
       <c r="S84" t="s">
         <v>38</v>
       </c>
       <c r="T84" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z84" t="s">
         <v>38</v>
       </c>
       <c r="AA84" s="2" t="s">
@@ -7381,7 +7879,7 @@
       </c>
       <c r="AC84">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD84">
         <v>1</v>
@@ -7396,11 +7894,11 @@
       </c>
       <c r="C85">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E85" t="s">
         <v>121</v>
@@ -7420,6 +7918,9 @@
       <c r="M85" t="s">
         <v>337</v>
       </c>
+      <c r="N85" t="s">
+        <v>38</v>
+      </c>
       <c r="O85" t="s">
         <v>321</v>
       </c>
@@ -7428,17 +7929,20 @@
       </c>
       <c r="Q85">
         <f t="shared" ca="1" si="7"/>
-        <v>9596</v>
+        <v>6702</v>
       </c>
       <c r="R85">
         <f t="shared" ca="1" si="8"/>
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="S85" t="s">
         <v>38</v>
       </c>
       <c r="T85" s="1">
         <v>15011</v>
+      </c>
+      <c r="Z85" t="s">
+        <v>38</v>
       </c>
       <c r="AA85" s="2" t="s">
         <v>38</v>
@@ -7463,11 +7967,11 @@
       </c>
       <c r="C86">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E86" t="s">
         <v>122</v>
@@ -7487,6 +7991,9 @@
       <c r="M86" t="s">
         <v>338</v>
       </c>
+      <c r="N86" t="s">
+        <v>38</v>
+      </c>
       <c r="O86" t="s">
         <v>322</v>
       </c>
@@ -7495,16 +8002,19 @@
       </c>
       <c r="Q86">
         <f t="shared" ca="1" si="7"/>
-        <v>7345</v>
+        <v>1764</v>
       </c>
       <c r="R86">
         <f t="shared" ca="1" si="8"/>
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="S86" t="s">
         <v>38</v>
       </c>
       <c r="T86" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z86" t="s">
         <v>38</v>
       </c>
       <c r="AA86" s="2" t="s">
@@ -7530,7 +8040,7 @@
       </c>
       <c r="C87">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="6"/>
@@ -7554,6 +8064,9 @@
       <c r="M87" t="s">
         <v>339</v>
       </c>
+      <c r="N87" t="s">
+        <v>38</v>
+      </c>
       <c r="O87" t="s">
         <v>323</v>
       </c>
@@ -7562,16 +8075,19 @@
       </c>
       <c r="Q87">
         <f t="shared" ca="1" si="7"/>
-        <v>6060</v>
+        <v>8659</v>
       </c>
       <c r="R87">
         <f t="shared" ca="1" si="8"/>
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="S87" t="s">
         <v>38</v>
       </c>
       <c r="T87" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z87" t="s">
         <v>38</v>
       </c>
       <c r="AA87" s="2" t="s">
@@ -7582,7 +8098,7 @@
       </c>
       <c r="AC87">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD87">
         <v>1</v>
@@ -7597,7 +8113,7 @@
       </c>
       <c r="C88">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D88">
         <f t="shared" ca="1" si="6"/>
@@ -7621,6 +8137,9 @@
       <c r="M88" t="s">
         <v>340</v>
       </c>
+      <c r="N88" t="s">
+        <v>38</v>
+      </c>
       <c r="O88" t="s">
         <v>324</v>
       </c>
@@ -7629,16 +8148,19 @@
       </c>
       <c r="Q88">
         <f t="shared" ca="1" si="7"/>
-        <v>7193</v>
+        <v>8396</v>
       </c>
       <c r="R88">
         <f t="shared" ca="1" si="8"/>
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="S88" t="s">
         <v>38</v>
       </c>
       <c r="T88" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z88" t="s">
         <v>38</v>
       </c>
       <c r="AA88" s="2" t="s">
@@ -7649,7 +8171,7 @@
       </c>
       <c r="AC88">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD88">
         <v>1</v>
@@ -7664,11 +8186,11 @@
       </c>
       <c r="C89">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D89">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E89" t="s">
         <v>125</v>
@@ -7688,6 +8210,9 @@
       <c r="M89" t="s">
         <v>341</v>
       </c>
+      <c r="N89" t="s">
+        <v>38</v>
+      </c>
       <c r="O89" t="s">
         <v>325</v>
       </c>
@@ -7696,11 +8221,11 @@
       </c>
       <c r="Q89">
         <f t="shared" ca="1" si="7"/>
-        <v>7880</v>
+        <v>2577</v>
       </c>
       <c r="R89">
         <f t="shared" ca="1" si="8"/>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="S89" t="s">
         <v>38</v>
@@ -7708,6 +8233,9 @@
       <c r="T89" s="1">
         <v>27610</v>
       </c>
+      <c r="Z89" t="s">
+        <v>38</v>
+      </c>
       <c r="AA89" s="2">
         <v>29825</v>
       </c>
@@ -7716,7 +8244,7 @@
       </c>
       <c r="AC89">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD89">
         <v>1</v>
@@ -7731,11 +8259,11 @@
       </c>
       <c r="C90">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E90" t="s">
         <v>126</v>
@@ -7755,6 +8283,9 @@
       <c r="M90" t="s">
         <v>342</v>
       </c>
+      <c r="N90" t="s">
+        <v>38</v>
+      </c>
       <c r="O90" t="s">
         <v>326</v>
       </c>
@@ -7763,17 +8294,20 @@
       </c>
       <c r="Q90">
         <f t="shared" ca="1" si="7"/>
-        <v>644</v>
+        <v>3454</v>
       </c>
       <c r="R90">
         <f t="shared" ca="1" si="8"/>
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="S90" t="s">
         <v>38</v>
       </c>
       <c r="T90" s="1">
         <v>27609</v>
+      </c>
+      <c r="Z90" t="s">
+        <v>38</v>
       </c>
       <c r="AA90" s="2" t="s">
         <v>38</v>
@@ -7798,11 +8332,11 @@
       </c>
       <c r="C91">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E91" t="s">
         <v>127</v>
@@ -7822,6 +8356,9 @@
       <c r="M91" t="s">
         <v>343</v>
       </c>
+      <c r="N91" t="s">
+        <v>38</v>
+      </c>
       <c r="O91" t="s">
         <v>327</v>
       </c>
@@ -7830,16 +8367,19 @@
       </c>
       <c r="Q91">
         <f t="shared" ca="1" si="7"/>
-        <v>4081</v>
+        <v>3746</v>
       </c>
       <c r="R91">
         <f t="shared" ca="1" si="8"/>
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="S91" t="s">
         <v>38</v>
       </c>
       <c r="T91" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z91" t="s">
         <v>38</v>
       </c>
       <c r="AA91" s="2" t="s">
@@ -7850,7 +8390,7 @@
       </c>
       <c r="AC91">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD91">
         <v>1</v>
@@ -7865,11 +8405,11 @@
       </c>
       <c r="C92">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D92">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E92" t="s">
         <v>128</v>
@@ -7889,6 +8429,9 @@
       <c r="M92" t="s">
         <v>344</v>
       </c>
+      <c r="N92" t="s">
+        <v>38</v>
+      </c>
       <c r="O92" t="s">
         <v>328</v>
       </c>
@@ -7897,17 +8440,20 @@
       </c>
       <c r="Q92">
         <f t="shared" ca="1" si="7"/>
-        <v>2656</v>
+        <v>1750</v>
       </c>
       <c r="R92">
         <f t="shared" ca="1" si="8"/>
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="S92" t="s">
         <v>38</v>
       </c>
       <c r="T92" s="1">
         <v>27752</v>
+      </c>
+      <c r="Z92" t="s">
+        <v>38</v>
       </c>
       <c r="AA92" s="2" t="s">
         <v>38</v>
@@ -7932,11 +8478,11 @@
       </c>
       <c r="C93">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D93">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E93" t="s">
         <v>129</v>
@@ -7956,6 +8502,9 @@
       <c r="M93" t="s">
         <v>345</v>
       </c>
+      <c r="N93" t="s">
+        <v>38</v>
+      </c>
       <c r="O93" t="s">
         <v>329</v>
       </c>
@@ -7964,16 +8513,19 @@
       </c>
       <c r="Q93">
         <f t="shared" ca="1" si="7"/>
-        <v>197</v>
+        <v>2711</v>
       </c>
       <c r="R93">
         <f t="shared" ca="1" si="8"/>
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="S93" t="s">
         <v>38</v>
       </c>
       <c r="T93" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z93" t="s">
         <v>38</v>
       </c>
       <c r="AA93" s="2" t="s">
@@ -7999,11 +8551,11 @@
       </c>
       <c r="C94">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D94">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E94" t="s">
         <v>130</v>
@@ -8023,6 +8575,9 @@
       <c r="M94" t="s">
         <v>346</v>
       </c>
+      <c r="N94" t="s">
+        <v>38</v>
+      </c>
       <c r="O94" t="s">
         <v>330</v>
       </c>
@@ -8031,16 +8586,19 @@
       </c>
       <c r="Q94">
         <f t="shared" ca="1" si="7"/>
-        <v>2942</v>
+        <v>6608</v>
       </c>
       <c r="R94">
         <f t="shared" ca="1" si="8"/>
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="S94" t="s">
         <v>38</v>
       </c>
       <c r="T94" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z94" t="s">
         <v>38</v>
       </c>
       <c r="AA94" s="2" t="s">
@@ -8051,7 +8609,7 @@
       </c>
       <c r="AC94">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD94">
         <v>1</v>
@@ -8066,11 +8624,11 @@
       </c>
       <c r="C95">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D95">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E95" t="s">
         <v>131</v>
@@ -8090,6 +8648,9 @@
       <c r="M95" t="s">
         <v>347</v>
       </c>
+      <c r="N95" t="s">
+        <v>38</v>
+      </c>
       <c r="O95" t="s">
         <v>331</v>
       </c>
@@ -8098,16 +8659,19 @@
       </c>
       <c r="Q95">
         <f t="shared" ca="1" si="7"/>
-        <v>280</v>
+        <v>9691</v>
       </c>
       <c r="R95">
         <f t="shared" ca="1" si="8"/>
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="S95" t="s">
         <v>38</v>
       </c>
       <c r="T95" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z95" t="s">
         <v>38</v>
       </c>
       <c r="AA95" s="2" t="s">
@@ -8133,11 +8697,11 @@
       </c>
       <c r="C96">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D96">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E96" t="s">
         <v>132</v>
@@ -8157,6 +8721,9 @@
       <c r="M96" t="s">
         <v>348</v>
       </c>
+      <c r="N96" t="s">
+        <v>38</v>
+      </c>
       <c r="O96" t="s">
         <v>332</v>
       </c>
@@ -8165,16 +8732,19 @@
       </c>
       <c r="Q96">
         <f t="shared" ca="1" si="7"/>
-        <v>9459</v>
+        <v>6471</v>
       </c>
       <c r="R96">
         <f t="shared" ca="1" si="8"/>
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="S96" t="s">
         <v>38</v>
       </c>
       <c r="T96" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z96" t="s">
         <v>38</v>
       </c>
       <c r="AA96" s="2" t="s">
@@ -8185,7 +8755,7 @@
       </c>
       <c r="AC96">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD96">
         <v>1</v>
@@ -8200,7 +8770,7 @@
       </c>
       <c r="C97">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D97">
         <f t="shared" ca="1" si="6"/>
@@ -8224,6 +8794,9 @@
       <c r="M97" t="s">
         <v>349</v>
       </c>
+      <c r="N97" t="s">
+        <v>38</v>
+      </c>
       <c r="O97" t="s">
         <v>333</v>
       </c>
@@ -8232,16 +8805,19 @@
       </c>
       <c r="Q97">
         <f t="shared" ca="1" si="7"/>
-        <v>6152</v>
+        <v>793</v>
       </c>
       <c r="R97">
         <f t="shared" ca="1" si="8"/>
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="S97" t="s">
         <v>38</v>
       </c>
       <c r="T97" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z97" t="s">
         <v>38</v>
       </c>
       <c r="AA97" s="2">
@@ -8252,7 +8828,7 @@
       </c>
       <c r="AC97">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD97">
         <v>1</v>
@@ -8267,11 +8843,11 @@
       </c>
       <c r="C98">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E98" t="s">
         <v>134</v>
@@ -8291,6 +8867,9 @@
       <c r="M98" t="s">
         <v>334</v>
       </c>
+      <c r="N98" t="s">
+        <v>38</v>
+      </c>
       <c r="O98" t="s">
         <v>337</v>
       </c>
@@ -8299,16 +8878,19 @@
       </c>
       <c r="Q98">
         <f t="shared" ca="1" si="7"/>
-        <v>5815</v>
+        <v>5608</v>
       </c>
       <c r="R98">
         <f t="shared" ca="1" si="8"/>
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="S98" t="s">
         <v>38</v>
       </c>
       <c r="T98" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z98" t="s">
         <v>38</v>
       </c>
       <c r="AA98" s="2" t="s">
@@ -8319,7 +8901,7 @@
       </c>
       <c r="AC98">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD98">
         <v>1</v>
@@ -8334,11 +8916,11 @@
       </c>
       <c r="C99">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D99">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E99" t="s">
         <v>135</v>
@@ -8358,6 +8940,9 @@
       <c r="M99" t="s">
         <v>335</v>
       </c>
+      <c r="N99" t="s">
+        <v>38</v>
+      </c>
       <c r="O99" t="s">
         <v>338</v>
       </c>
@@ -8366,11 +8951,11 @@
       </c>
       <c r="Q99">
         <f t="shared" ca="1" si="7"/>
-        <v>6592</v>
+        <v>2103</v>
       </c>
       <c r="R99">
         <f t="shared" ca="1" si="8"/>
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="S99" t="s">
         <v>38</v>
@@ -8378,6 +8963,9 @@
       <c r="T99" s="1">
         <v>27622</v>
       </c>
+      <c r="Z99" t="s">
+        <v>38</v>
+      </c>
       <c r="AA99" s="2">
         <v>29901</v>
       </c>
@@ -8386,7 +8974,7 @@
       </c>
       <c r="AC99">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD99">
         <v>1</v>
@@ -8401,11 +8989,11 @@
       </c>
       <c r="C100">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D100">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E100" t="s">
         <v>136</v>
@@ -8425,6 +9013,9 @@
       <c r="M100" t="s">
         <v>336</v>
       </c>
+      <c r="N100" t="s">
+        <v>38</v>
+      </c>
       <c r="O100" t="s">
         <v>339</v>
       </c>
@@ -8433,17 +9024,20 @@
       </c>
       <c r="Q100">
         <f t="shared" ca="1" si="7"/>
-        <v>7380</v>
+        <v>5168</v>
       </c>
       <c r="R100">
         <f t="shared" ca="1" si="8"/>
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="S100" t="s">
         <v>38</v>
       </c>
       <c r="T100" s="1">
         <v>27365</v>
+      </c>
+      <c r="Z100" t="s">
+        <v>38</v>
       </c>
       <c r="AA100" s="2">
         <v>30462</v>
@@ -8468,7 +9062,7 @@
       </c>
       <c r="C101">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D101">
         <f t="shared" ca="1" si="6"/>
@@ -8492,6 +9086,9 @@
       <c r="M101" t="s">
         <v>327</v>
       </c>
+      <c r="N101" t="s">
+        <v>38</v>
+      </c>
       <c r="O101" t="s">
         <v>340</v>
       </c>
@@ -8500,11 +9097,11 @@
       </c>
       <c r="Q101">
         <f t="shared" ca="1" si="7"/>
-        <v>3475</v>
+        <v>5942</v>
       </c>
       <c r="R101">
         <f t="shared" ca="1" si="8"/>
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="S101" t="s">
         <v>38</v>
@@ -8512,6 +9109,9 @@
       <c r="T101" s="1">
         <v>23067</v>
       </c>
+      <c r="Z101" t="s">
+        <v>38</v>
+      </c>
       <c r="AA101" s="2">
         <v>30454</v>
       </c>
@@ -8520,7 +9120,7 @@
       </c>
       <c r="AC101">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD101">
         <v>1</v>

</xml_diff>

<commit_message>
carga db y modificaciones en raiz
</commit_message>
<xml_diff>
--- a/Excel/Carga DB Postgres/Ingreso - cargado.xlsx
+++ b/Excel/Carga DB Postgres/Ingreso - cargado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="363">
   <si>
     <t>fechahora</t>
   </si>
@@ -1099,6 +1099,12 @@
   </si>
   <si>
     <t>BMF687</t>
+  </si>
+  <si>
+    <t>estitular</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -1433,10 +1439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG121"/>
+  <dimension ref="A1:AH121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AH96" sqref="AH96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1458,7 +1464,7 @@
     <col min="24" max="24" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:34">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1558,8 +1564,11 @@
       <c r="AG1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:33">
+      <c r="AH1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1638,8 +1647,11 @@
       <c r="AG2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:33">
+      <c r="AH2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -1718,8 +1730,11 @@
       <c r="AG3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:33">
+      <c r="AH3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -1795,8 +1810,11 @@
       <c r="AG4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:33">
+      <c r="AH4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
       <c r="A5" t="s">
         <v>194</v>
       </c>
@@ -1875,8 +1893,11 @@
       <c r="AG5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:33">
+      <c r="AH5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -1953,7 +1974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:34">
       <c r="A7" t="s">
         <v>196</v>
       </c>
@@ -2032,8 +2053,11 @@
       <c r="AG7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:33">
+      <c r="AH7" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34">
       <c r="A8" t="s">
         <v>197</v>
       </c>
@@ -2109,8 +2133,11 @@
       <c r="AG8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:33">
+      <c r="AH8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34">
       <c r="A9" t="s">
         <v>198</v>
       </c>
@@ -2189,8 +2216,11 @@
       <c r="AG9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:33">
+      <c r="AH9" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34">
       <c r="A10" t="s">
         <v>199</v>
       </c>
@@ -2266,8 +2296,11 @@
       <c r="AG10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:33">
+      <c r="AH10" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34">
       <c r="A11" t="s">
         <v>200</v>
       </c>
@@ -2346,8 +2379,11 @@
       <c r="AG11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:33">
+      <c r="AH11" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34">
       <c r="A12" t="s">
         <v>201</v>
       </c>
@@ -2423,8 +2459,11 @@
       <c r="AG12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:33">
+      <c r="AH12" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34">
       <c r="A13" t="s">
         <v>202</v>
       </c>
@@ -2503,8 +2542,11 @@
       <c r="AG13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:33">
+      <c r="AH13" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34">
       <c r="A14" t="s">
         <v>203</v>
       </c>
@@ -2583,8 +2625,11 @@
       <c r="AG14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:33">
+      <c r="AH14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34">
       <c r="A15" t="s">
         <v>204</v>
       </c>
@@ -2660,8 +2705,11 @@
       <c r="AG15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:33">
+      <c r="AH15" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34">
       <c r="A16" t="s">
         <v>205</v>
       </c>
@@ -2735,7 +2783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:34">
       <c r="A17" t="s">
         <v>206</v>
       </c>
@@ -2811,8 +2859,11 @@
       <c r="AG17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:33">
+      <c r="AH17" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34">
       <c r="A18" t="s">
         <v>207</v>
       </c>
@@ -2891,8 +2942,11 @@
       <c r="AG18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:33">
+      <c r="AH18" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34">
       <c r="A19" t="s">
         <v>208</v>
       </c>
@@ -2971,8 +3025,11 @@
       <c r="AG19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:33">
+      <c r="AH19" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34">
       <c r="A20" t="s">
         <v>209</v>
       </c>
@@ -3051,8 +3108,11 @@
       <c r="AG20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:33">
+      <c r="AH20" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34">
       <c r="A21" t="s">
         <v>210</v>
       </c>
@@ -3131,8 +3191,11 @@
       <c r="AG21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:33">
+      <c r="AH21" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34">
       <c r="A22" t="s">
         <v>211</v>
       </c>
@@ -3208,8 +3271,11 @@
       <c r="AG22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:33">
+      <c r="AH22" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34">
       <c r="A23" t="s">
         <v>212</v>
       </c>
@@ -3285,8 +3351,11 @@
       <c r="AG23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:33">
+      <c r="AH23" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34">
       <c r="A24" t="s">
         <v>213</v>
       </c>
@@ -3365,8 +3434,11 @@
       <c r="AG24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:33">
+      <c r="AH24" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34">
       <c r="A25" t="s">
         <v>214</v>
       </c>
@@ -3442,8 +3514,11 @@
       <c r="AG25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:33">
+      <c r="AH25" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34">
       <c r="A26" t="s">
         <v>215</v>
       </c>
@@ -3520,7 +3595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:34">
       <c r="A27" t="s">
         <v>216</v>
       </c>
@@ -3599,8 +3674,11 @@
       <c r="AG27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:33">
+      <c r="AH27" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34">
       <c r="A28" t="s">
         <v>217</v>
       </c>
@@ -3679,8 +3757,11 @@
       <c r="AG28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:33">
+      <c r="AH28" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34">
       <c r="A29" t="s">
         <v>218</v>
       </c>
@@ -3759,8 +3840,11 @@
       <c r="AG29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:33">
+      <c r="AH29" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34">
       <c r="A30" t="s">
         <v>219</v>
       </c>
@@ -3839,8 +3923,11 @@
       <c r="AG30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:33">
+      <c r="AH30" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34">
       <c r="A31" t="s">
         <v>220</v>
       </c>
@@ -3919,8 +4006,11 @@
       <c r="AG31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:33">
+      <c r="AH31" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34">
       <c r="A32" t="s">
         <v>221</v>
       </c>
@@ -3996,8 +4086,11 @@
       <c r="AG32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:33">
+      <c r="AH32" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34">
       <c r="A33" t="s">
         <v>222</v>
       </c>
@@ -4076,8 +4169,11 @@
       <c r="AG33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:33">
+      <c r="AH33" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34">
       <c r="A34" t="s">
         <v>223</v>
       </c>
@@ -4156,8 +4252,11 @@
       <c r="AG34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:33">
+      <c r="AH34" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34">
       <c r="A35" t="s">
         <v>333</v>
       </c>
@@ -4236,8 +4335,11 @@
       <c r="AG35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:33">
+      <c r="AH35" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34">
       <c r="A36" t="s">
         <v>224</v>
       </c>
@@ -4314,7 +4416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:34">
       <c r="A37" t="s">
         <v>225</v>
       </c>
@@ -4393,8 +4495,11 @@
       <c r="AG37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:33">
+      <c r="AH37" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="38" spans="1:34">
       <c r="A38" t="s">
         <v>226</v>
       </c>
@@ -4473,8 +4578,11 @@
       <c r="AG38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:33">
+      <c r="AH38" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34">
       <c r="A39" t="s">
         <v>227</v>
       </c>
@@ -4553,8 +4661,11 @@
       <c r="AG39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:33">
+      <c r="AH39" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="40" spans="1:34">
       <c r="A40" t="s">
         <v>228</v>
       </c>
@@ -4633,8 +4744,11 @@
       <c r="AG40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:33">
+      <c r="AH40" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34">
       <c r="A41" t="s">
         <v>229</v>
       </c>
@@ -4713,8 +4827,11 @@
       <c r="AG41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:33">
+      <c r="AH41" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34">
       <c r="A42" t="s">
         <v>230</v>
       </c>
@@ -4793,8 +4910,11 @@
       <c r="AG42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:33">
+      <c r="AH42" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -4873,8 +4993,11 @@
       <c r="AG43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:33">
+      <c r="AH43" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34">
       <c r="A44" t="s">
         <v>232</v>
       </c>
@@ -4950,8 +5073,11 @@
       <c r="AG44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:33">
+      <c r="AH44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34">
       <c r="A45" t="s">
         <v>233</v>
       </c>
@@ -5030,8 +5156,11 @@
       <c r="AG45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:33">
+      <c r="AH45" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34">
       <c r="A46" t="s">
         <v>234</v>
       </c>
@@ -5105,7 +5234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:34">
       <c r="A47" t="s">
         <v>235</v>
       </c>
@@ -5181,8 +5310,11 @@
       <c r="AG47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:33">
+      <c r="AH47" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34">
       <c r="A48" t="s">
         <v>236</v>
       </c>
@@ -5261,8 +5393,11 @@
       <c r="AG48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:33">
+      <c r="AH48" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="49" spans="1:34">
       <c r="A49" t="s">
         <v>237</v>
       </c>
@@ -5341,8 +5476,11 @@
       <c r="AG49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:33">
+      <c r="AH49" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="50" spans="1:34">
       <c r="A50" t="s">
         <v>238</v>
       </c>
@@ -5421,8 +5559,11 @@
       <c r="AG50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:33">
+      <c r="AH50" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="51" spans="1:34">
       <c r="A51" t="s">
         <v>239</v>
       </c>
@@ -5501,8 +5642,11 @@
       <c r="AG51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:33">
+      <c r="AH51" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="52" spans="1:34">
       <c r="A52" t="s">
         <v>240</v>
       </c>
@@ -5581,8 +5725,11 @@
       <c r="AG52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:33">
+      <c r="AH52" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="53" spans="1:34">
       <c r="A53" t="s">
         <v>241</v>
       </c>
@@ -5661,8 +5808,11 @@
       <c r="AG53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:33">
+      <c r="AH53" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="54" spans="1:34">
       <c r="A54" t="s">
         <v>242</v>
       </c>
@@ -5741,8 +5891,11 @@
       <c r="AG54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:33">
+      <c r="AH54" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="55" spans="1:34">
       <c r="A55" t="s">
         <v>243</v>
       </c>
@@ -5818,8 +5971,11 @@
       <c r="AG55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:33">
+      <c r="AH55" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="56" spans="1:34">
       <c r="A56" t="s">
         <v>244</v>
       </c>
@@ -5896,7 +6052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:34">
       <c r="A57" t="s">
         <v>245</v>
       </c>
@@ -5975,8 +6131,11 @@
       <c r="AG57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:33">
+      <c r="AH57" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="58" spans="1:34">
       <c r="A58" t="s">
         <v>246</v>
       </c>
@@ -6055,8 +6214,11 @@
       <c r="AG58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:33">
+      <c r="AH58" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="59" spans="1:34">
       <c r="A59" t="s">
         <v>247</v>
       </c>
@@ -6135,8 +6297,11 @@
       <c r="AG59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:33">
+      <c r="AH59" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="60" spans="1:34">
       <c r="A60" t="s">
         <v>248</v>
       </c>
@@ -6212,8 +6377,11 @@
       <c r="AG60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:33">
+      <c r="AH60" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="61" spans="1:34">
       <c r="A61" t="s">
         <v>249</v>
       </c>
@@ -6292,8 +6460,11 @@
       <c r="AG61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:33">
+      <c r="AH61" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="62" spans="1:34">
       <c r="A62" t="s">
         <v>250</v>
       </c>
@@ -6378,8 +6549,11 @@
       <c r="AG62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:33">
+      <c r="AH62" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="63" spans="1:34">
       <c r="A63" t="s">
         <v>251</v>
       </c>
@@ -6464,8 +6638,11 @@
       <c r="AG63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:33">
+      <c r="AH63" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="64" spans="1:34">
       <c r="A64" t="s">
         <v>252</v>
       </c>
@@ -6550,8 +6727,11 @@
       <c r="AG64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:33">
+      <c r="AH64" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="65" spans="1:34">
       <c r="A65" t="s">
         <v>253</v>
       </c>
@@ -6633,8 +6813,11 @@
       <c r="AG65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:33">
+      <c r="AH65" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="66" spans="1:34">
       <c r="A66" t="s">
         <v>254</v>
       </c>
@@ -6717,7 +6900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:34">
       <c r="A67" t="s">
         <v>255</v>
       </c>
@@ -6802,8 +6985,11 @@
       <c r="AG67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:33">
+      <c r="AH67" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="68" spans="1:34">
       <c r="A68" t="s">
         <v>256</v>
       </c>
@@ -6888,8 +7074,11 @@
       <c r="AG68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:33">
+      <c r="AH68" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="69" spans="1:34">
       <c r="A69" t="s">
         <v>257</v>
       </c>
@@ -6974,8 +7163,11 @@
       <c r="AG69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:33">
+      <c r="AH69" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="70" spans="1:34">
       <c r="A70" t="s">
         <v>258</v>
       </c>
@@ -7057,8 +7249,11 @@
       <c r="AG70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:33">
+      <c r="AH70" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="71" spans="1:34">
       <c r="A71" t="s">
         <v>259</v>
       </c>
@@ -7143,8 +7338,11 @@
       <c r="AG71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:33">
+      <c r="AH71" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="72" spans="1:34">
       <c r="A72" t="s">
         <v>260</v>
       </c>
@@ -7223,8 +7421,11 @@
       <c r="AG72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:33">
+      <c r="AH72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="73" spans="1:34">
       <c r="A73" t="s">
         <v>261</v>
       </c>
@@ -7303,8 +7504,11 @@
       <c r="AG73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:33">
+      <c r="AH73" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="74" spans="1:34">
       <c r="A74" t="s">
         <v>262</v>
       </c>
@@ -7383,8 +7587,11 @@
       <c r="AG74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:33">
+      <c r="AH74" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="75" spans="1:34">
       <c r="A75" t="s">
         <v>263</v>
       </c>
@@ -7463,8 +7670,11 @@
       <c r="AG75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:33">
+      <c r="AH75" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:34">
       <c r="A76" t="s">
         <v>264</v>
       </c>
@@ -7538,7 +7748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:33">
+    <row r="77" spans="1:34">
       <c r="A77" t="s">
         <v>265</v>
       </c>
@@ -7617,8 +7827,11 @@
       <c r="AG77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:33">
+      <c r="AH77" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="78" spans="1:34">
       <c r="A78" t="s">
         <v>266</v>
       </c>
@@ -7697,8 +7910,11 @@
       <c r="AG78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:33">
+      <c r="AH78" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="79" spans="1:34">
       <c r="A79" t="s">
         <v>267</v>
       </c>
@@ -7777,8 +7993,11 @@
       <c r="AG79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:33">
+      <c r="AH79" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="80" spans="1:34">
       <c r="A80" t="s">
         <v>268</v>
       </c>
@@ -7857,8 +8076,11 @@
       <c r="AG80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:33">
+      <c r="AH80" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="81" spans="1:34">
       <c r="A81" t="s">
         <v>269</v>
       </c>
@@ -7937,8 +8159,11 @@
       <c r="AG81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:33">
+      <c r="AH81" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="82" spans="1:34">
       <c r="A82" t="s">
         <v>270</v>
       </c>
@@ -8017,8 +8242,11 @@
       <c r="AG82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:33">
+      <c r="AH82" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="83" spans="1:34">
       <c r="A83" t="s">
         <v>271</v>
       </c>
@@ -8097,8 +8325,11 @@
       <c r="AG83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:33">
+      <c r="AH83" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="84" spans="1:34">
       <c r="A84" t="s">
         <v>272</v>
       </c>
@@ -8177,8 +8408,11 @@
       <c r="AG84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:33">
+      <c r="AH84" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="85" spans="1:34">
       <c r="A85" t="s">
         <v>273</v>
       </c>
@@ -8257,8 +8491,11 @@
       <c r="AG85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:33">
+      <c r="AH85" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="86" spans="1:34">
       <c r="A86" t="s">
         <v>274</v>
       </c>
@@ -8335,7 +8572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:33">
+    <row r="87" spans="1:34">
       <c r="A87" t="s">
         <v>275</v>
       </c>
@@ -8414,8 +8651,11 @@
       <c r="AG87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:33">
+      <c r="AH87" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="88" spans="1:34">
       <c r="A88" t="s">
         <v>276</v>
       </c>
@@ -8491,8 +8731,11 @@
       <c r="AG88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:33">
+      <c r="AH88" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="89" spans="1:34">
       <c r="A89" t="s">
         <v>277</v>
       </c>
@@ -8571,8 +8814,11 @@
       <c r="AG89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:33">
+      <c r="AH89" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="90" spans="1:34">
       <c r="A90" t="s">
         <v>278</v>
       </c>
@@ -8651,8 +8897,11 @@
       <c r="AG90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:33">
+      <c r="AH90" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="91" spans="1:34">
       <c r="A91" t="s">
         <v>279</v>
       </c>
@@ -8731,8 +8980,11 @@
       <c r="AG91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:33">
+      <c r="AH91" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="92" spans="1:34">
       <c r="A92" t="s">
         <v>280</v>
       </c>
@@ -8811,8 +9063,11 @@
       <c r="AG92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:33">
+      <c r="AH92" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="93" spans="1:34">
       <c r="A93" t="s">
         <v>281</v>
       </c>
@@ -8891,8 +9146,11 @@
       <c r="AG93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:33">
+      <c r="AH93" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="94" spans="1:34">
       <c r="A94" t="s">
         <v>282</v>
       </c>
@@ -8971,8 +9229,11 @@
       <c r="AG94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:33">
+      <c r="AH94" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="95" spans="1:34">
       <c r="A95" t="s">
         <v>283</v>
       </c>
@@ -9048,8 +9309,11 @@
       <c r="AG95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:33">
+      <c r="AH95" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="96" spans="1:34">
       <c r="A96" t="s">
         <v>284</v>
       </c>
@@ -9123,7 +9387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:33">
+    <row r="97" spans="1:34">
       <c r="A97" t="s">
         <v>285</v>
       </c>
@@ -9202,8 +9466,11 @@
       <c r="AG97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:33">
+      <c r="AH97" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="98" spans="1:34">
       <c r="A98" t="s">
         <v>286</v>
       </c>
@@ -9282,8 +9549,11 @@
       <c r="AG98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:33">
+      <c r="AH98" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="99" spans="1:34">
       <c r="A99" t="s">
         <v>287</v>
       </c>
@@ -9362,8 +9632,11 @@
       <c r="AG99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:33">
+      <c r="AH99" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="100" spans="1:34">
       <c r="A100" t="s">
         <v>288</v>
       </c>
@@ -9442,8 +9715,11 @@
       <c r="AG100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:33">
+      <c r="AH100" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="101" spans="1:34">
       <c r="A101" t="s">
         <v>289</v>
       </c>
@@ -9522,8 +9798,11 @@
       <c r="AG101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:33">
+      <c r="AH101" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="102" spans="1:34">
       <c r="A102" t="s">
         <v>334</v>
       </c>
@@ -9602,8 +9881,11 @@
       <c r="AG102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:33">
+      <c r="AH102" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="103" spans="1:34">
       <c r="A103" t="s">
         <v>335</v>
       </c>
@@ -9682,8 +9964,11 @@
       <c r="AG103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:33">
+      <c r="AH103" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="104" spans="1:34">
       <c r="A104" t="s">
         <v>336</v>
       </c>
@@ -9762,8 +10047,11 @@
       <c r="AG104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:33">
+      <c r="AH104" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="105" spans="1:34">
       <c r="A105" t="s">
         <v>337</v>
       </c>
@@ -9842,8 +10130,11 @@
       <c r="AG105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:33">
+      <c r="AH105" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="106" spans="1:34">
       <c r="A106" t="s">
         <v>338</v>
       </c>
@@ -9922,8 +10213,11 @@
       <c r="AG106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:33">
+      <c r="AH106" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="107" spans="1:34">
       <c r="A107" t="s">
         <v>339</v>
       </c>
@@ -10002,8 +10296,11 @@
       <c r="AG107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:33">
+      <c r="AH107" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="108" spans="1:34">
       <c r="A108" t="s">
         <v>340</v>
       </c>
@@ -10082,8 +10379,11 @@
       <c r="AG108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:33">
+      <c r="AH108" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="109" spans="1:34">
       <c r="A109" t="s">
         <v>341</v>
       </c>
@@ -10162,8 +10462,11 @@
       <c r="AG109">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:33">
+      <c r="AH109" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="110" spans="1:34">
       <c r="A110" t="s">
         <v>342</v>
       </c>
@@ -10242,8 +10545,11 @@
       <c r="AG110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:33">
+      <c r="AH110" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="111" spans="1:34">
       <c r="A111" t="s">
         <v>343</v>
       </c>
@@ -10322,8 +10628,11 @@
       <c r="AG111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:33">
+      <c r="AH111" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="112" spans="1:34">
       <c r="A112" t="s">
         <v>344</v>
       </c>
@@ -10402,8 +10711,11 @@
       <c r="AG112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:33">
+      <c r="AH112" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="113" spans="1:34">
       <c r="A113" t="s">
         <v>345</v>
       </c>
@@ -10482,8 +10794,11 @@
       <c r="AG113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:33">
+      <c r="AH113" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="114" spans="1:34">
       <c r="A114" t="s">
         <v>346</v>
       </c>
@@ -10562,8 +10877,11 @@
       <c r="AG114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:33">
+      <c r="AH114" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="115" spans="1:34">
       <c r="A115" t="s">
         <v>347</v>
       </c>
@@ -10642,8 +10960,11 @@
       <c r="AG115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:33">
+      <c r="AH115" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="116" spans="1:34">
       <c r="A116" t="s">
         <v>348</v>
       </c>
@@ -10722,8 +11043,11 @@
       <c r="AG116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:33">
+      <c r="AH116" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="117" spans="1:34">
       <c r="A117" t="s">
         <v>349</v>
       </c>
@@ -10802,8 +11126,11 @@
       <c r="AG117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:33">
+      <c r="AH117" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="118" spans="1:34">
       <c r="A118" t="s">
         <v>350</v>
       </c>
@@ -10882,8 +11209,11 @@
       <c r="AG118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:33">
+      <c r="AH118" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="119" spans="1:34">
       <c r="A119" t="s">
         <v>351</v>
       </c>
@@ -10962,8 +11292,11 @@
       <c r="AG119">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:33">
+      <c r="AH119" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="120" spans="1:34">
       <c r="A120" t="s">
         <v>352</v>
       </c>
@@ -11042,8 +11375,11 @@
       <c r="AG120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:33">
+      <c r="AH120" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="121" spans="1:34">
       <c r="A121" t="s">
         <v>353</v>
       </c>
@@ -11121,6 +11457,9 @@
       </c>
       <c r="AG121">
         <v>1</v>
+      </c>
+      <c r="AH121" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
casos de prueba: 136 escenarios
</commit_message>
<xml_diff>
--- a/Excel/Carga DB Postgres/Ingreso - cargado.xlsx
+++ b/Excel/Carga DB Postgres/Ingreso - cargado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="370">
   <si>
     <t>fechahora</t>
   </si>
@@ -1114,6 +1114,18 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>2017-09-25-20:09:58</t>
+  </si>
+  <si>
+    <t>2017-10-30-13:22:46</t>
+  </si>
+  <si>
+    <t>ESTA-DOCU</t>
+  </si>
+  <si>
+    <t>ALCO-DOCU</t>
   </si>
 </sst>
 </file>
@@ -1448,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH123"/>
+  <dimension ref="A1:AH125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AE116" sqref="AE116"/>
+    <sheetView tabSelected="1" topLeftCell="E95" workbookViewId="0">
+      <selection activeCell="J125" sqref="J125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -11670,6 +11682,172 @@
         <v>5</v>
       </c>
       <c r="AH123" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="124" spans="1:34">
+      <c r="A124" t="s">
+        <v>366</v>
+      </c>
+      <c r="B124">
+        <v>3</v>
+      </c>
+      <c r="C124">
+        <v>5</v>
+      </c>
+      <c r="D124" t="s">
+        <v>57</v>
+      </c>
+      <c r="E124" t="s">
+        <v>126</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G124" t="s">
+        <v>33</v>
+      </c>
+      <c r="J124" t="s">
+        <v>368</v>
+      </c>
+      <c r="K124" t="s">
+        <v>296</v>
+      </c>
+      <c r="L124" t="s">
+        <v>37</v>
+      </c>
+      <c r="M124" t="s">
+        <v>311</v>
+      </c>
+      <c r="N124" t="s">
+        <v>313</v>
+      </c>
+      <c r="O124">
+        <v>8540</v>
+      </c>
+      <c r="P124">
+        <v>21</v>
+      </c>
+      <c r="Q124">
+        <v>39</v>
+      </c>
+      <c r="R124">
+        <v>25</v>
+      </c>
+      <c r="S124" t="s">
+        <v>37</v>
+      </c>
+      <c r="T124">
+        <v>1</v>
+      </c>
+      <c r="U124" s="1">
+        <v>16855456</v>
+      </c>
+      <c r="AA124">
+        <v>16017888</v>
+      </c>
+      <c r="AB124">
+        <v>16085667</v>
+      </c>
+      <c r="AC124">
+        <v>565699</v>
+      </c>
+      <c r="AD124">
+        <v>680669</v>
+      </c>
+      <c r="AE124" t="s">
+        <v>362</v>
+      </c>
+      <c r="AF124">
+        <v>1</v>
+      </c>
+      <c r="AG124">
+        <v>1</v>
+      </c>
+      <c r="AH124" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="125" spans="1:34">
+      <c r="A125" t="s">
+        <v>367</v>
+      </c>
+      <c r="B125">
+        <v>3</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+      <c r="D125" t="s">
+        <v>58</v>
+      </c>
+      <c r="E125" t="s">
+        <v>123</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G125" t="s">
+        <v>35</v>
+      </c>
+      <c r="J125" t="s">
+        <v>369</v>
+      </c>
+      <c r="K125" t="s">
+        <v>297</v>
+      </c>
+      <c r="L125" t="s">
+        <v>37</v>
+      </c>
+      <c r="M125" t="s">
+        <v>312</v>
+      </c>
+      <c r="N125" t="s">
+        <v>314</v>
+      </c>
+      <c r="O125">
+        <v>3606</v>
+      </c>
+      <c r="P125">
+        <v>22</v>
+      </c>
+      <c r="Q125">
+        <v>40</v>
+      </c>
+      <c r="R125">
+        <v>146</v>
+      </c>
+      <c r="S125" t="s">
+        <v>37</v>
+      </c>
+      <c r="T125">
+        <v>1</v>
+      </c>
+      <c r="U125" s="1">
+        <v>16855456</v>
+      </c>
+      <c r="AA125">
+        <v>16017888</v>
+      </c>
+      <c r="AB125">
+        <v>16085667</v>
+      </c>
+      <c r="AC125">
+        <v>565699</v>
+      </c>
+      <c r="AD125">
+        <v>680669</v>
+      </c>
+      <c r="AE125" t="s">
+        <v>362</v>
+      </c>
+      <c r="AF125">
+        <v>1</v>
+      </c>
+      <c r="AG125">
+        <v>1</v>
+      </c>
+      <c r="AH125" t="s">
         <v>362</v>
       </c>
     </row>

</xml_diff>